<commit_message>
tweak PX1224, PX1228 deadlines
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B71A93BC-42E5-41AC-B525-42BC89F89980}"/>
+  <xr:revisionPtr revIDLastSave="606" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C384DBA-4A76-4992-9D41-C04B8BEAB2BC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="328">
   <si>
     <t>Module Code</t>
   </si>
@@ -1024,6 +1024,9 @@
   <si>
     <t>Su?</t>
   </si>
+  <si>
+    <t>AstroPhotograph</t>
+  </si>
 </sst>
 </file>
 
@@ -1129,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1273,21 +1276,6 @@
     <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1349,24 +1337,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri (Body)"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3284,6 +3254,24 @@
         <name val="Calibri (Body)"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -8903,7 +8891,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9369,40 +9357,40 @@
     </tableColumn>
     <tableColumn id="30" xr3:uid="{82DD5B5B-C808-4E6E-849C-7A03DC6D0B69}" name="Description" dataDxfId="94"/>
     <tableColumn id="36" xr3:uid="{A7BF30F6-C808-4B8F-B3FF-9FAF20E2145A}" name="Summative" dataDxfId="93"/>
-    <tableColumn id="37" xr3:uid="{F2060C32-39B6-4ADB-B712-F0770A906BCC}" name="Day of Week" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{E6637FEB-7F23-45F0-99D2-96D20DD2DAEF}" name="Duration" dataDxfId="92"/>
-    <tableColumn id="31" xr3:uid="{FD1E9614-3960-4F72-BD42-711A4CC7BBA0}" name="Nominal Hours" dataDxfId="91">
+    <tableColumn id="37" xr3:uid="{F2060C32-39B6-4ADB-B712-F0770A906BCC}" name="Day of Week" dataDxfId="92"/>
+    <tableColumn id="16" xr3:uid="{E6637FEB-7F23-45F0-99D2-96D20DD2DAEF}" name="Duration" dataDxfId="91"/>
+    <tableColumn id="31" xr3:uid="{FD1E9614-3960-4F72-BD42-711A4CC7BBA0}" name="Nominal Hours" dataDxfId="90">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]])*4*Table1[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{E11C773A-511F-4D25-8636-C56C5B61ED90}" name="Hours" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{04E38F13-8347-412C-866C-6EFE6796253C}" name="Autumn Week 1" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{254D6A24-FC1B-44C7-A3DF-52DA2A250D31}" name="Autumn Week 2" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{9EB326C3-772E-4E56-89FB-BA3A00291293}" name="Autumn Week 3" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{94BC6C78-5A89-4267-B1C1-BFA70E5A9F34}" name="Autumn Week 4" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{CF3B6389-B559-4FE3-8B33-FEDB303382B1}" name="Autumn Week 5" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{8DD80B9C-D1B1-4CDE-A624-4CD3A15113DD}" name="Autumn Week 6" dataDxfId="84"/>
-    <tableColumn id="10" xr3:uid="{8C4EBEE4-01CB-4AD0-B594-F466CC36D370}" name="Autumn Week 7" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{7F8C91DE-BE61-47CF-A916-D06ED7B283E9}" name="Autumn Week 8" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{9D58139A-0F96-4203-8D22-58BC34744B87}" name="Autumn Week 9" dataDxfId="81"/>
-    <tableColumn id="13" xr3:uid="{43C545DF-9B9E-4080-8012-F9EFA0F01283}" name="Autumn Week 10" dataDxfId="80"/>
-    <tableColumn id="14" xr3:uid="{829AB976-2AB2-435C-8F11-DE08DACA4407}" name="Autumn Week 11" dataDxfId="79"/>
-    <tableColumn id="15" xr3:uid="{9126A0EA-FC34-4876-9D56-A0AC39C5526C}" name="Autumn Week 12" dataDxfId="78"/>
-    <tableColumn id="17" xr3:uid="{15B891EE-FCC8-4E53-A90D-3E10FFC1E9FA}" name="Spring Week 1" dataDxfId="77"/>
-    <tableColumn id="18" xr3:uid="{464CA212-3B53-4678-AFE4-8AF8308C1986}" name="Spring Week 2" dataDxfId="76"/>
-    <tableColumn id="19" xr3:uid="{B560E823-CC29-418C-B26C-52D9FFC8C72E}" name="Spring Week 3" dataDxfId="75"/>
-    <tableColumn id="20" xr3:uid="{D95606F3-E0A0-4907-91E0-4AD09D0C65CB}" name="Spring Week 4" dataDxfId="74"/>
-    <tableColumn id="21" xr3:uid="{E71FF892-9A4B-444C-8972-62D92F81B0E7}" name="Spring Week 5" dataDxfId="73"/>
-    <tableColumn id="22" xr3:uid="{C7775BA8-178A-4501-A8DE-2B2CF77A2451}" name="Spring Week 6" dataDxfId="72"/>
-    <tableColumn id="23" xr3:uid="{51A89A97-F839-4F50-88A9-65049D65C9B0}" name="Spring Week 7" dataDxfId="71"/>
-    <tableColumn id="24" xr3:uid="{26EE6D10-4FC4-49AE-8DE6-18AC556C293D}" name="Spring Week 8" dataDxfId="70"/>
-    <tableColumn id="25" xr3:uid="{FCB1B9FB-21DA-415A-86E6-C8E14F864E1B}" name="Spring Week 9" dataDxfId="69"/>
-    <tableColumn id="26" xr3:uid="{54402AE1-DC77-41BA-BCC7-28BCA7186B44}" name="Spring Week 10" dataDxfId="68"/>
-    <tableColumn id="27" xr3:uid="{31C092D1-BD77-4126-8E72-8E74D0D11509}" name="Spring Week 11" dataDxfId="67"/>
-    <tableColumn id="28" xr3:uid="{56D67770-E36A-46FE-97FA-76CD24229C51}" name="Spring Week 12" dataDxfId="66"/>
-    <tableColumn id="29" xr3:uid="{785AD842-5ED0-4E27-B4B7-26E6FF9AC266}" name="Sub-total" dataDxfId="65">
+    <tableColumn id="32" xr3:uid="{E11C773A-511F-4D25-8636-C56C5B61ED90}" name="Hours" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{04E38F13-8347-412C-866C-6EFE6796253C}" name="Autumn Week 1" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{254D6A24-FC1B-44C7-A3DF-52DA2A250D31}" name="Autumn Week 2" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{9EB326C3-772E-4E56-89FB-BA3A00291293}" name="Autumn Week 3" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{94BC6C78-5A89-4267-B1C1-BFA70E5A9F34}" name="Autumn Week 4" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{CF3B6389-B559-4FE3-8B33-FEDB303382B1}" name="Autumn Week 5" dataDxfId="84"/>
+    <tableColumn id="9" xr3:uid="{8DD80B9C-D1B1-4CDE-A624-4CD3A15113DD}" name="Autumn Week 6" dataDxfId="83"/>
+    <tableColumn id="10" xr3:uid="{8C4EBEE4-01CB-4AD0-B594-F466CC36D370}" name="Autumn Week 7" dataDxfId="82"/>
+    <tableColumn id="11" xr3:uid="{7F8C91DE-BE61-47CF-A916-D06ED7B283E9}" name="Autumn Week 8" dataDxfId="81"/>
+    <tableColumn id="12" xr3:uid="{9D58139A-0F96-4203-8D22-58BC34744B87}" name="Autumn Week 9" dataDxfId="80"/>
+    <tableColumn id="13" xr3:uid="{43C545DF-9B9E-4080-8012-F9EFA0F01283}" name="Autumn Week 10" dataDxfId="79"/>
+    <tableColumn id="14" xr3:uid="{829AB976-2AB2-435C-8F11-DE08DACA4407}" name="Autumn Week 11" dataDxfId="78"/>
+    <tableColumn id="15" xr3:uid="{9126A0EA-FC34-4876-9D56-A0AC39C5526C}" name="Autumn Week 12" dataDxfId="77"/>
+    <tableColumn id="17" xr3:uid="{15B891EE-FCC8-4E53-A90D-3E10FFC1E9FA}" name="Spring Week 1" dataDxfId="76"/>
+    <tableColumn id="18" xr3:uid="{464CA212-3B53-4678-AFE4-8AF8308C1986}" name="Spring Week 2" dataDxfId="75"/>
+    <tableColumn id="19" xr3:uid="{B560E823-CC29-418C-B26C-52D9FFC8C72E}" name="Spring Week 3" dataDxfId="74"/>
+    <tableColumn id="20" xr3:uid="{D95606F3-E0A0-4907-91E0-4AD09D0C65CB}" name="Spring Week 4" dataDxfId="73"/>
+    <tableColumn id="21" xr3:uid="{E71FF892-9A4B-444C-8972-62D92F81B0E7}" name="Spring Week 5" dataDxfId="72"/>
+    <tableColumn id="22" xr3:uid="{C7775BA8-178A-4501-A8DE-2B2CF77A2451}" name="Spring Week 6" dataDxfId="71"/>
+    <tableColumn id="23" xr3:uid="{51A89A97-F839-4F50-88A9-65049D65C9B0}" name="Spring Week 7" dataDxfId="70"/>
+    <tableColumn id="24" xr3:uid="{26EE6D10-4FC4-49AE-8DE6-18AC556C293D}" name="Spring Week 8" dataDxfId="69"/>
+    <tableColumn id="25" xr3:uid="{FCB1B9FB-21DA-415A-86E6-C8E14F864E1B}" name="Spring Week 9" dataDxfId="68"/>
+    <tableColumn id="26" xr3:uid="{54402AE1-DC77-41BA-BCC7-28BCA7186B44}" name="Spring Week 10" dataDxfId="67"/>
+    <tableColumn id="27" xr3:uid="{31C092D1-BD77-4126-8E72-8E74D0D11509}" name="Spring Week 11" dataDxfId="66"/>
+    <tableColumn id="28" xr3:uid="{56D67770-E36A-46FE-97FA-76CD24229C51}" name="Spring Week 12" dataDxfId="65"/>
+    <tableColumn id="29" xr3:uid="{785AD842-5ED0-4E27-B4B7-26E6FF9AC266}" name="Sub-total" dataDxfId="64">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{EE5D0E71-7823-4EE2-9CC1-32BF500AB742}" name="Total Hours" dataDxfId="64">
+    <tableColumn id="35" xr3:uid="{EE5D0E71-7823-4EE2-9CC1-32BF500AB742}" name="Total Hours" dataDxfId="63">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9411,49 +9399,49 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A071F52D-AD51-4120-94C5-67D4117EBD07}" name="Table14" displayName="Table14" ref="A1:AE64" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A071F52D-AD51-4120-94C5-67D4117EBD07}" name="Table14" displayName="Table14" ref="A1:AE64" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="A1:AE64" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD64">
     <sortCondition ref="A1:A132"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{D7CE4D57-09F4-4B9D-B464-A087075D1C39}" name="Module Code" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{DE2920B2-70AC-48F3-99E7-07B70BC1E928}" name="Module Title" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{61946E7A-4C82-425B-89A6-3DBD530FCD55}" name="Contact type" dataDxfId="56"/>
-    <tableColumn id="34" xr3:uid="{55A68E2B-9324-4E9E-9629-6611EC7C904E}" name="Credits" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{D7CE4D57-09F4-4B9D-B464-A087075D1C39}" name="Module Code" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{DE2920B2-70AC-48F3-99E7-07B70BC1E928}" name="Module Title" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{61946E7A-4C82-425B-89A6-3DBD530FCD55}" name="Contact type" dataDxfId="55"/>
+    <tableColumn id="34" xr3:uid="{55A68E2B-9324-4E9E-9629-6611EC7C904E}" name="Credits" dataDxfId="54">
       <calculatedColumnFormula>INDEX(Table2[Credits],MATCH(Table14[[#This Row],[Module Code]],Table2[Module Code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{9C4C2C35-CE5A-4469-93FA-21FC6F57EDAD}" name="Semester" dataDxfId="54">
+    <tableColumn id="30" xr3:uid="{9C4C2C35-CE5A-4469-93FA-21FC6F57EDAD}" name="Semester" dataDxfId="53">
       <calculatedColumnFormula>INDEX(Table2[Semester],MATCH(Table14[[#This Row],[Module Code]],Table2[Module Code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{A7B09E14-0C35-459D-A9D0-5143D8AFFE4E}" name="Nominal Hours" dataDxfId="53">
+    <tableColumn id="31" xr3:uid="{A7B09E14-0C35-459D-A9D0-5143D8AFFE4E}" name="Nominal Hours" dataDxfId="52">
       <calculatedColumnFormula>INDEX(Table2[Contact Time],MATCH(Table14[[#This Row],[Module Code]],Table2[Module Code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{503822B3-8862-4FCD-9DD3-3B52F57A97BE}" name="Autumn Week 1" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{760391D0-3219-4B11-8E3D-3E00EEDFA9DD}" name="Autumn Week 2" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{6EE5E3E9-C4FB-49BE-932C-B84EA0A7970D}" name="Autumn Week 3" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{2C7AD515-480E-49A6-8076-95205ACF95EC}" name="Autumn Week 4" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{6FD8C5C6-433E-493B-BB28-5ADD15CFC7FB}" name="Autumn Week 5" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{801E6BE2-75F8-40A5-A263-0AAEFDAA63E7}" name="Autumn Week 6" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{976D463A-C6BC-4636-B732-53E6CDF3F6C7}" name="Autumn Week 7" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{D025F987-6302-4D7B-9A9A-636F867D1872}" name="Autumn Week 8" dataDxfId="45"/>
-    <tableColumn id="12" xr3:uid="{D30D10EE-2DE5-4659-AA67-2134D11D6119}" name="Autumn Week 9" dataDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{35E8F713-2D13-47B7-9811-293DA89F0D62}" name="Autumn Week 10" dataDxfId="43"/>
-    <tableColumn id="14" xr3:uid="{5DD48606-F817-4B30-8BA1-A96457CBB489}" name="Autumn Week 11" dataDxfId="42"/>
-    <tableColumn id="15" xr3:uid="{9B982ED1-A4C5-4E87-99AB-70713F2B634E}" name="Autumn Week 12" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{3AFDFF11-D351-428A-AC16-E674EB9DD7CC}" name="Spring Week 1" dataDxfId="40"/>
-    <tableColumn id="18" xr3:uid="{1431E9F9-328E-4229-9377-39D94C660D67}" name="Spring Week 2" dataDxfId="39"/>
-    <tableColumn id="19" xr3:uid="{8E1051DB-2A93-4ABA-8317-8F9921CF483D}" name="Spring Week 3" dataDxfId="38"/>
-    <tableColumn id="20" xr3:uid="{98B745E4-C481-42FF-9D3B-0D0899BD3DB6}" name="Spring Week 4" dataDxfId="37"/>
-    <tableColumn id="21" xr3:uid="{2FC9B562-4622-444D-9372-5637BFE48E0A}" name="Spring Week 5" dataDxfId="36"/>
-    <tableColumn id="22" xr3:uid="{95778D77-82F1-4B00-8FED-6FEB2BF83C3D}" name="Spring Week 6" dataDxfId="35"/>
-    <tableColumn id="23" xr3:uid="{9A49A64C-9A09-47A0-BC65-A8C1C98DACA3}" name="Spring Week 7" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{191AACBA-3CF0-48E5-B522-FCD2CCE9AC99}" name="Spring Week 8" dataDxfId="33"/>
-    <tableColumn id="25" xr3:uid="{DC35B6C1-904B-4E6A-A04F-ADF850A50D85}" name="Spring Week 9" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{BEB9E86A-57BF-4A1E-A499-BADB9EAD1DE9}" name="Spring Week 10" dataDxfId="31"/>
-    <tableColumn id="27" xr3:uid="{D640FB81-F093-4E3F-B7A1-6995DDDD6305}" name="Spring Week 11" dataDxfId="30"/>
-    <tableColumn id="28" xr3:uid="{496FDC17-F0F2-4381-96DA-177DC578A786}" name="Spring Week 12" dataDxfId="29"/>
-    <tableColumn id="32" xr3:uid="{65BCC67A-5DC9-4957-BB42-BCF5FCA71B17}" name="Total" dataDxfId="28">
+    <tableColumn id="4" xr3:uid="{503822B3-8862-4FCD-9DD3-3B52F57A97BE}" name="Autumn Week 1" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{760391D0-3219-4B11-8E3D-3E00EEDFA9DD}" name="Autumn Week 2" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{6EE5E3E9-C4FB-49BE-932C-B84EA0A7970D}" name="Autumn Week 3" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{2C7AD515-480E-49A6-8076-95205ACF95EC}" name="Autumn Week 4" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{6FD8C5C6-433E-493B-BB28-5ADD15CFC7FB}" name="Autumn Week 5" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{801E6BE2-75F8-40A5-A263-0AAEFDAA63E7}" name="Autumn Week 6" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{976D463A-C6BC-4636-B732-53E6CDF3F6C7}" name="Autumn Week 7" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{D025F987-6302-4D7B-9A9A-636F867D1872}" name="Autumn Week 8" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{D30D10EE-2DE5-4659-AA67-2134D11D6119}" name="Autumn Week 9" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{35E8F713-2D13-47B7-9811-293DA89F0D62}" name="Autumn Week 10" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{5DD48606-F817-4B30-8BA1-A96457CBB489}" name="Autumn Week 11" dataDxfId="41"/>
+    <tableColumn id="15" xr3:uid="{9B982ED1-A4C5-4E87-99AB-70713F2B634E}" name="Autumn Week 12" dataDxfId="40"/>
+    <tableColumn id="17" xr3:uid="{3AFDFF11-D351-428A-AC16-E674EB9DD7CC}" name="Spring Week 1" dataDxfId="39"/>
+    <tableColumn id="18" xr3:uid="{1431E9F9-328E-4229-9377-39D94C660D67}" name="Spring Week 2" dataDxfId="38"/>
+    <tableColumn id="19" xr3:uid="{8E1051DB-2A93-4ABA-8317-8F9921CF483D}" name="Spring Week 3" dataDxfId="37"/>
+    <tableColumn id="20" xr3:uid="{98B745E4-C481-42FF-9D3B-0D0899BD3DB6}" name="Spring Week 4" dataDxfId="36"/>
+    <tableColumn id="21" xr3:uid="{2FC9B562-4622-444D-9372-5637BFE48E0A}" name="Spring Week 5" dataDxfId="35"/>
+    <tableColumn id="22" xr3:uid="{95778D77-82F1-4B00-8FED-6FEB2BF83C3D}" name="Spring Week 6" dataDxfId="34"/>
+    <tableColumn id="23" xr3:uid="{9A49A64C-9A09-47A0-BC65-A8C1C98DACA3}" name="Spring Week 7" dataDxfId="33"/>
+    <tableColumn id="24" xr3:uid="{191AACBA-3CF0-48E5-B522-FCD2CCE9AC99}" name="Spring Week 8" dataDxfId="32"/>
+    <tableColumn id="25" xr3:uid="{DC35B6C1-904B-4E6A-A04F-ADF850A50D85}" name="Spring Week 9" dataDxfId="31"/>
+    <tableColumn id="26" xr3:uid="{BEB9E86A-57BF-4A1E-A499-BADB9EAD1DE9}" name="Spring Week 10" dataDxfId="30"/>
+    <tableColumn id="27" xr3:uid="{D640FB81-F093-4E3F-B7A1-6995DDDD6305}" name="Spring Week 11" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{496FDC17-F0F2-4381-96DA-177DC578A786}" name="Spring Week 12" dataDxfId="28"/>
+    <tableColumn id="32" xr3:uid="{65BCC67A-5DC9-4957-BB42-BCF5FCA71B17}" name="Total" dataDxfId="27">
       <calculatedColumnFormula>SUM(Table14[[#This Row],[Autumn Week 1]:[Spring Week 12]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9462,37 +9450,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4070B5A2-579F-42D6-AF31-642FC3F016DD}" name="Table2" displayName="Table2" ref="A1:W100" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4070B5A2-579F-42D6-AF31-642FC3F016DD}" name="Table2" displayName="Table2" ref="A1:W100" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25">
   <autoFilter ref="A1:W100" xr:uid="{4070B5A2-579F-42D6-AF31-642FC3F016DD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B62">
     <sortCondition ref="A1:A62"/>
   </sortState>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{A36A2B86-0F30-4188-9ECD-AE5BC71A59F4}" name="Module Code" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{D3F20037-EF35-4207-A530-484E1EB45719}" name="Module Title" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{40C22022-10B9-411F-9B76-B89140ABFFB2}" name="Alternative Module Code" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{CB12E405-1802-457C-AF17-F1B9CB3BBF13}" name="Source" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{EA737976-1AA7-49B6-8752-A388621554F4}" name="Semester" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{16DFC84F-5858-467D-B447-49992D721E4B}" name="Level" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{A17BC4BA-A3CB-442D-9BDC-D3B41B98B389}" name="Credits" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{FD7ED610-D6EC-4B93-B979-1E6C071D4AB2}" name="AllUG" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{7E25B4F4-1A7D-48D9-AAA2-AF5C97240797}" name="Physics" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{A36A2B86-0F30-4188-9ECD-AE5BC71A59F4}" name="Module Code" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{D3F20037-EF35-4207-A530-484E1EB45719}" name="Module Title" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{40C22022-10B9-411F-9B76-B89140ABFFB2}" name="Alternative Module Code" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{CB12E405-1802-457C-AF17-F1B9CB3BBF13}" name="Source" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{EA737976-1AA7-49B6-8752-A388621554F4}" name="Semester" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{16DFC84F-5858-467D-B447-49992D721E4B}" name="Level" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{A17BC4BA-A3CB-442D-9BDC-D3B41B98B389}" name="Credits" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{FD7ED610-D6EC-4B93-B979-1E6C071D4AB2}" name="AllUG" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{7E25B4F4-1A7D-48D9-AAA2-AF5C97240797}" name="Physics" dataDxfId="15"/>
     <tableColumn id="17" xr3:uid="{AA3AE96F-2651-49D7-89AD-BA94806438AE}" name="PhysAstro"/>
-    <tableColumn id="4" xr3:uid="{9C7DD469-E550-411F-8467-246A1543FB38}" name="Astro" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{3C5D3AEB-487E-4678-A42F-BE4BA4D0E9AA}" name="MedPhys" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{9C7DD469-E550-411F-8467-246A1543FB38}" name="Astro" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{3C5D3AEB-487E-4678-A42F-BE4BA4D0E9AA}" name="MedPhys" dataDxfId="13"/>
     <tableColumn id="23" xr3:uid="{AF3E1EB3-2B73-43ED-85E9-1E8314E0F50D}" name="AllPG"/>
-    <tableColumn id="14" xr3:uid="{AE552873-9B31-41A6-B73C-D052477CA74C}" name="MScPhysics" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{8F51CE76-3A29-487A-A13C-FB63C79CF3E6}" name="MScAstro" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{443DB830-B47F-48D9-93EC-9DDA5086534B}" name="MScDataPhys" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{228F99C6-6D58-4321-9F11-706B965FD631}" name="MScDataAstro" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{AE552873-9B31-41A6-B73C-D052477CA74C}" name="MScPhysics" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{8F51CE76-3A29-487A-A13C-FB63C79CF3E6}" name="MScAstro" dataDxfId="11"/>
+    <tableColumn id="19" xr3:uid="{443DB830-B47F-48D9-93EC-9DDA5086534B}" name="MScDataPhys" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{228F99C6-6D58-4321-9F11-706B965FD631}" name="MScDataAstro" dataDxfId="9"/>
     <tableColumn id="18" xr3:uid="{10668F71-1EDF-482E-86A5-46E1F3C15120}" name="MScCSPhysics"/>
     <tableColumn id="21" xr3:uid="{3CC5C4CC-6537-4363-AB9D-6A0F69456D30}" name="CDTCSPhysics"/>
     <tableColumn id="16" xr3:uid="{DB790F5F-BEF0-41CE-A68A-1AA9DF83D66B}" name="Contact Time"/>
-    <tableColumn id="10" xr3:uid="{60774AFA-B365-4EB5-AAFF-6235868F8C97}" name="Exam Weight (%)" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{537B7C75-E9C0-42F2-9F3C-6E960AB2D257}" name="CA weight" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{60774AFA-B365-4EB5-AAFF-6235868F8C97}" name="Exam Weight (%)" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{537B7C75-E9C0-42F2-9F3C-6E960AB2D257}" name="CA weight" dataDxfId="7">
       <calculatedColumnFormula>100-Table2[[#This Row],[Exam Weight (%)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{75DA2527-5A08-4ECE-B4E4-752A8F8BF059}" name="CA Check" dataDxfId="7">
+    <tableColumn id="11" xr3:uid="{75DA2527-5A08-4ECE-B4E4-752A8F8BF059}" name="CA Check" dataDxfId="6">
       <calculatedColumnFormula>IF(COUNTIF(Table1[Module Code],Table2[[#This Row],[Module Code]])&gt;0,SUMIFS(Table1[Sub-total],Table1[Module Code],Table2[[#This Row],[Module Code]],Table1[Summative],"Y")*100,SUMIFS(Table1[Sub-total],Table1[Module Code],Table2[[#This Row],[Alternative Module Code]],Table1[Summative],"Y")*100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9820,27 +9808,27 @@
   <dimension ref="A1:AK157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H153" sqref="H153"/>
+      <selection pane="bottomRight" activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.796875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.7265625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.7265625" style="10" customWidth="1"/>
-    <col min="12" max="23" width="9.08984375" style="14" customWidth="1"/>
-    <col min="24" max="35" width="9.08984375" style="16"/>
+    <col min="6" max="6" width="21.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.73046875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.73046875" style="10" customWidth="1"/>
+    <col min="12" max="23" width="9.06640625" style="14" customWidth="1"/>
+    <col min="24" max="35" width="9.06640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="44" customFormat="1" ht="29">
+    <row r="1" spans="1:37" s="44" customFormat="1" ht="28.5">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -10978,7 +10966,7 @@
         <v>234</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="I15" s="11">
         <v>2</v>
@@ -11011,13 +10999,13 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
       <c r="AF15" s="20"/>
-      <c r="AG15" s="45">
-        <v>0.3</v>
-      </c>
+      <c r="AG15" s="20"/>
       <c r="AH15" s="46">
         <v>-0.3</v>
       </c>
-      <c r="AI15" s="20"/>
+      <c r="AI15" s="45">
+        <v>0.3</v>
+      </c>
       <c r="AJ15" s="27">
         <f>SUM(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]])</f>
         <v>0</v>
@@ -11184,34 +11172,34 @@
       <c r="B18" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="52">
+      <c r="D18" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>30</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F18" s="51" t="s">
-        <v>307</v>
+      <c r="F18" s="12" t="s">
+        <v>327</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="I18" s="53">
+        <v>322</v>
+      </c>
+      <c r="I18" s="11">
         <v>4</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>4</v>
-      </c>
-      <c r="K18" s="53"/>
+        <v>-18</v>
+      </c>
+      <c r="K18" s="11"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
@@ -11233,18 +11221,20 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
       <c r="AF18" s="20"/>
-      <c r="AG18" s="20"/>
-      <c r="AH18" s="20"/>
-      <c r="AI18" s="20">
+      <c r="AG18" s="45">
         <v>0.1</v>
       </c>
-      <c r="AJ18" s="55">
+      <c r="AH18" s="46">
+        <v>-1</v>
+      </c>
+      <c r="AI18" s="20"/>
+      <c r="AJ18" s="27">
         <f>SUM(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]])</f>
-        <v>0.1</v>
-      </c>
-      <c r="AK18" s="55">
+        <v>-0.9</v>
+      </c>
+      <c r="AK18" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>4</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="19" spans="1:37">
@@ -21751,16 +21741,16 @@
       <selection pane="bottomRight" activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.796875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="10" customWidth="1"/>
-    <col min="7" max="15" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="8.7265625" style="16"/>
+    <col min="6" max="6" width="10.73046875" style="10" customWidth="1"/>
+    <col min="7" max="15" width="16.265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="17.265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="8.73046875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -27910,14 +27900,14 @@
       <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.796875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.796875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.265625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="5" customWidth="1"/>
   </cols>
@@ -28345,7 +28335,7 @@
       </c>
       <c r="W8">
         <f>IF(COUNTIF(Table1[Module Code],Table2[[#This Row],[Module Code]])&gt;0,SUMIFS(Table1[Sub-total],Table1[Module Code],Table2[[#This Row],[Module Code]],Table1[Summative],"Y")*100,SUMIFS(Table1[Sub-total],Table1[Module Code],Table2[[#This Row],[Alternative Module Code]],Table1[Summative],"Y")*100)</f>
-        <v>30.000000000000004</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -33340,11 +33330,11 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -33520,7 +33510,7 @@
       </c>
       <c r="C10">
         <f>SUMIF(Table1[Module Code],Sheet2!A10,Table1[Total Hours])</f>
-        <v>10.5</v>
+        <v>-11.5</v>
       </c>
       <c r="D10">
         <f>INDEX(Table14[Total],MATCH(Sheet2!A10,Table14[Module Code],0))</f>
@@ -33528,11 +33518,11 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>32.5</v>
+        <v>10.5</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>3.25</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="11" spans="1:6">

</xml_diff>

<commit_message>
edited deadlines to match timetable
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="715" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00C2773-A011-487D-80D5-9C245D55A718}"/>
+  <xr:revisionPtr revIDLastSave="932" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA6460C-967D-4E04-903E-5136AFB530AC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="49" r:id="rId5"/>
+    <pivotCache cacheId="19" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="346">
   <si>
     <t>Module Code</t>
   </si>
@@ -827,9 +827,6 @@
     <t>Online test</t>
   </si>
   <si>
-    <t>sessions (prep)</t>
-  </si>
-  <si>
     <t>Assignment</t>
   </si>
   <si>
@@ -837,12 +834,6 @@
   </si>
   <si>
     <t>Problem set</t>
-  </si>
-  <si>
-    <t>3min Pres</t>
-  </si>
-  <si>
-    <t>Group Pres</t>
   </si>
   <si>
     <t>Article</t>
@@ -855,9 +846,6 @@
   </si>
   <si>
     <t>Exercise 3</t>
-  </si>
-  <si>
-    <t>Poster Pres</t>
   </si>
   <si>
     <t>Class Test</t>
@@ -887,31 +875,10 @@
     <t>CA1</t>
   </si>
   <si>
-    <t>CA2 (*)</t>
-  </si>
-  <si>
     <t>Lab Diary (*)</t>
   </si>
   <si>
-    <t>CA (*)</t>
-  </si>
-  <si>
     <t>Presentation (*)</t>
-  </si>
-  <si>
-    <t>Assignment (*)</t>
-  </si>
-  <si>
-    <t>Final Report (*)</t>
-  </si>
-  <si>
-    <t>Final Diary (*)</t>
-  </si>
-  <si>
-    <t>Project Diary (*)</t>
-  </si>
-  <si>
-    <t>Project Report (*)</t>
   </si>
   <si>
     <t>ENT610</t>
@@ -962,22 +929,7 @@
     <t>CA 2</t>
   </si>
   <si>
-    <t>CA (TBC)</t>
-  </si>
-  <si>
-    <t>ML Project (TBC)</t>
-  </si>
-  <si>
-    <t>Class Test (TBC)</t>
-  </si>
-  <si>
-    <t>ML Methods (TBC)</t>
-  </si>
-  <si>
     <t>Abstract</t>
-  </si>
-  <si>
-    <t>Pres (+/- 1 week)</t>
   </si>
   <si>
     <t>AllUG</t>
@@ -998,28 +950,13 @@
     <t>Th</t>
   </si>
   <si>
-    <t>Presentation (Tutorial)</t>
-  </si>
-  <si>
     <t>(*)</t>
   </si>
   <si>
     <t>We</t>
   </si>
   <si>
-    <t>Pres</t>
-  </si>
-  <si>
     <t>Poster</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Su?</t>
-  </si>
-  <si>
-    <t>AstroPhotograph</t>
   </si>
   <si>
     <t>OA</t>
@@ -1028,13 +965,121 @@
     <t>Spring Exams</t>
   </si>
   <si>
-    <t>Viva</t>
+    <t>Fr</t>
   </si>
   <si>
-    <t>Weekly Tasks</t>
+    <t>Lab Report A</t>
   </si>
   <si>
-    <t>Reflections (*)</t>
+    <t>Lab Report B</t>
+  </si>
+  <si>
+    <t>Lab Report C</t>
+  </si>
+  <si>
+    <t>Pres (Tutorial) (*)</t>
+  </si>
+  <si>
+    <t>Data Analysis (*)</t>
+  </si>
+  <si>
+    <t>Workshop (*)</t>
+  </si>
+  <si>
+    <t>(TBC)</t>
+  </si>
+  <si>
+    <t>AstroPhoto (U/D)</t>
+  </si>
+  <si>
+    <t>CA2 (U/D)</t>
+  </si>
+  <si>
+    <t>Mo/Th</t>
+  </si>
+  <si>
+    <t>Assignment (U/D)</t>
+  </si>
+  <si>
+    <t>CA (U/D)</t>
+  </si>
+  <si>
+    <t>Reflections (U/D)</t>
+  </si>
+  <si>
+    <t>Presentation (U/D)</t>
+  </si>
+  <si>
+    <t>Poster Pres (*)</t>
+  </si>
+  <si>
+    <t>Th/Fr</t>
+  </si>
+  <si>
+    <t>Lab Diary (*) (U/D)</t>
+  </si>
+  <si>
+    <t>Workshops (*)</t>
+  </si>
+  <si>
+    <t>(Lab)</t>
+  </si>
+  <si>
+    <t>3min Pres (*)</t>
+  </si>
+  <si>
+    <t>Group Pres (*)</t>
+  </si>
+  <si>
+    <t>Lab Diary (P)</t>
+  </si>
+  <si>
+    <t>Weekly Tasks (P)</t>
+  </si>
+  <si>
+    <t>Workshop (P)</t>
+  </si>
+  <si>
+    <t>Pres (*) (+/- 1wk)</t>
+  </si>
+  <si>
+    <t>Final Diary (U/D)</t>
+  </si>
+  <si>
+    <t>Final Report (U/D)</t>
+  </si>
+  <si>
+    <t>Mo/We</t>
+  </si>
+  <si>
+    <t>Quiz (P)</t>
+  </si>
+  <si>
+    <t>Quiz (*)</t>
+  </si>
+  <si>
+    <t>Tu/Fr</t>
+  </si>
+  <si>
+    <t>Project Diary (U/D)</t>
+  </si>
+  <si>
+    <t>Project Report (U/D)</t>
+  </si>
+  <si>
+    <t>Viva (*)</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>ML Project</t>
+  </si>
+  <si>
+    <t>Class Test (*)</t>
+  </si>
+  <si>
+    <t>ML Methods</t>
   </si>
 </sst>
 </file>
@@ -8922,7 +8967,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="49" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9371,8 +9416,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}" name="Table1" displayName="Table1" ref="A1:AL159" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102" totalsRowBorderDxfId="101">
-  <autoFilter ref="A1:AL159" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}" name="Table1" displayName="Table1" ref="A1:AL160" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102" totalsRowBorderDxfId="101">
+  <autoFilter ref="A1:AL160" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI136">
     <sortCondition ref="A1:A136"/>
   </sortState>
@@ -9837,30 +9882,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66039B40-29AD-4D93-B125-EAF72A7B3996}">
-  <dimension ref="A1:AL159"/>
+  <dimension ref="A1:AL160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.73046875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.73046875" style="10" customWidth="1"/>
-    <col min="12" max="23" width="9.06640625" style="14" customWidth="1"/>
-    <col min="24" max="36" width="9.06640625" style="16"/>
+    <col min="6" max="6" width="21.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.7265625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7265625" style="10" customWidth="1"/>
+    <col min="12" max="23" width="9.08984375" style="14" customWidth="1"/>
+    <col min="24" max="36" width="9.08984375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="44" customFormat="1" ht="28.5">
+    <row r="1" spans="1:38" s="44" customFormat="1" ht="29">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -9883,7 +9928,7 @@
         <v>233</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="I1" s="40" t="s">
         <v>78</v>
@@ -9967,7 +10012,7 @@
         <v>177</v>
       </c>
       <c r="AJ1" s="42" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="AK1" s="43" t="s">
         <v>178</v>
@@ -10001,7 +10046,7 @@
         <v>234</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I2" s="11">
         <v>1</v>
@@ -10074,13 +10119,13 @@
         <v>20</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I3" s="11">
         <v>4</v>
@@ -10153,7 +10198,7 @@
         <v>234</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I4" s="11">
         <v>3</v>
@@ -10226,7 +10271,7 @@
         <v>234</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I5" s="11">
         <v>1</v>
@@ -10313,7 +10358,7 @@
         <v>234</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I6" s="11">
         <v>2</v>
@@ -10384,13 +10429,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I7" s="11">
         <v>3</v>
@@ -10461,7 +10506,7 @@
         <v>234</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I8" s="11">
         <v>3</v>
@@ -10526,13 +10571,13 @@
         <v>20</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>207</v>
+        <v>312</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="I9" s="11">
         <v>1</v>
@@ -10597,13 +10642,13 @@
         <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="I10" s="11">
         <v>2</v>
@@ -10686,7 +10731,7 @@
         <v>234</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I11" s="11">
         <v>3</v>
@@ -10759,7 +10804,7 @@
         <v>234</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I12" s="11">
         <v>4</v>
@@ -10844,13 +10889,13 @@
         <v>10</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>222</v>
+        <v>313</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="I13" s="11">
         <v>1</v>
@@ -10935,13 +10980,13 @@
         <v>10</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="I14" s="11">
         <v>3</v>
@@ -11008,13 +11053,13 @@
         <v>10</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I15" s="11">
         <v>2</v>
@@ -11089,7 +11134,7 @@
         <v>234</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I16" s="11">
         <v>1</v>
@@ -11164,13 +11209,13 @@
         <v>10</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="I17" s="11">
         <v>4</v>
@@ -11235,13 +11280,13 @@
         <v>10</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="I18" s="11">
         <v>4</v>
@@ -11314,7 +11359,7 @@
         <v>234</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I19" s="11">
         <v>2</v>
@@ -11385,13 +11430,13 @@
         <v>10</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I20" s="11">
         <v>6</v>
@@ -11462,7 +11507,7 @@
         <v>234</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I21" s="11">
         <v>6</v>
@@ -11533,7 +11578,7 @@
         <v>234</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="I22" s="11">
         <v>1</v>
@@ -11618,13 +11663,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>209</v>
+        <v>319</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="I23" s="11">
         <v>3</v>
@@ -11699,7 +11744,7 @@
         <v>234</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I24" s="11">
         <v>1</v>
@@ -11791,13 +11836,13 @@
         <v>10</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I25" s="11">
         <v>3</v>
@@ -11864,13 +11909,13 @@
         <v>10</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I26" s="11">
         <v>3</v>
@@ -11939,13 +11984,13 @@
         <v>10</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>207</v>
+        <v>312</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I27" s="11">
         <v>1</v>
@@ -12018,7 +12063,7 @@
         <v>234</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I28" s="11">
         <v>3</v>
@@ -12085,13 +12130,13 @@
         <v>10</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I29" s="11">
         <v>11</v>
@@ -12158,13 +12203,13 @@
         <v>10</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>222</v>
+        <v>331</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I30" s="11">
         <v>1</v>
@@ -12249,13 +12294,13 @@
         <v>10</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>285</v>
+        <v>318</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I31" s="11">
         <v>3</v>
@@ -12314,7 +12359,9 @@
       <c r="B32" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D32" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
@@ -12324,13 +12371,13 @@
         <v>10</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I32" s="11">
         <v>1</v>
@@ -12397,13 +12444,13 @@
         <v>10</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>283</v>
+        <v>319</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I33" s="11">
         <v>3</v>
@@ -12476,13 +12523,13 @@
         <v>10</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="I34" s="11">
         <v>1</v>
@@ -12572,13 +12619,13 @@
         <v>10</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I35" s="11">
         <v>2</v>
@@ -12649,13 +12696,13 @@
         <v>10</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>284</v>
+        <v>321</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I36" s="11">
         <v>3</v>
@@ -12730,7 +12777,7 @@
         <v>234</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I37" s="11">
         <v>9</v>
@@ -12797,13 +12844,13 @@
         <v>10</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>258</v>
+        <v>329</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="I38" s="11">
         <v>1</v>
@@ -12884,7 +12931,7 @@
         <v>234</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I39" s="11">
         <v>5</v>
@@ -12949,13 +12996,13 @@
         <v>20</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I40" s="11">
         <v>3</v>
@@ -13026,13 +13073,13 @@
         <v>20</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="G41" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I41" s="11">
         <v>3</v>
@@ -13109,13 +13156,13 @@
         <v>20</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>207</v>
+        <v>312</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I42" s="11">
         <v>1</v>
@@ -13182,13 +13229,13 @@
         <v>20</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G43" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I43" s="11">
         <v>11</v>
@@ -13261,7 +13308,7 @@
         <v>234</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I44" s="11">
         <v>4</v>
@@ -13334,7 +13381,7 @@
         <v>234</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="I45" s="11">
         <v>2</v>
@@ -13413,7 +13460,7 @@
         <v>234</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="I46" s="11">
         <v>2</v>
@@ -13484,7 +13531,7 @@
         <v>234</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I47" s="11">
         <v>3</v>
@@ -13557,7 +13604,7 @@
         <v>234</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I48" s="11">
         <v>6</v>
@@ -13628,7 +13675,7 @@
         <v>234</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I49" s="11">
         <v>1</v>
@@ -13719,7 +13766,7 @@
         <v>234</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I50" s="11">
         <v>3</v>
@@ -13788,13 +13835,13 @@
         <v>10</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G51" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I51" s="11">
         <v>1</v>
@@ -13869,7 +13916,7 @@
         <v>234</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I52" s="11">
         <v>1</v>
@@ -13960,7 +14007,7 @@
         <v>234</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I53" s="11">
         <v>4</v>
@@ -14025,13 +14072,13 @@
         <v>10</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="G54" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I54" s="11">
         <v>4</v>
@@ -14096,13 +14143,13 @@
         <v>10</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
       <c r="G55" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I55" s="11">
         <v>1</v>
@@ -14189,7 +14236,7 @@
         <v>234</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I56" s="11">
         <v>6</v>
@@ -14254,13 +14301,13 @@
         <v>10</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G57" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I57" s="11">
         <v>1</v>
@@ -14327,13 +14374,13 @@
         <v>10</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G58" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I58" s="11">
         <v>9</v>
@@ -14398,13 +14445,13 @@
         <v>10</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
       <c r="G59" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I59" s="11">
         <v>1</v>
@@ -14491,7 +14538,7 @@
         <v>234</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I60" s="11">
         <v>6</v>
@@ -14556,13 +14603,13 @@
         <v>10</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G61" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I61" s="11">
         <v>1</v>
@@ -14629,13 +14676,13 @@
         <v>10</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I62" s="11">
         <v>1</v>
@@ -14706,7 +14753,7 @@
         <v>234</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I63" s="11">
         <v>1</v>
@@ -14797,7 +14844,7 @@
         <v>234</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I64" s="11">
         <v>4</v>
@@ -14868,7 +14915,7 @@
         <v>234</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I65" s="13">
         <v>1</v>
@@ -14966,7 +15013,7 @@
         <v>234</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I66" s="11">
         <v>1</v>
@@ -15053,7 +15100,7 @@
         <v>234</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I67" s="11">
         <v>4</v>
@@ -15128,7 +15175,7 @@
         <v>234</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I68" s="11">
         <v>4</v>
@@ -15201,7 +15248,7 @@
         <v>234</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I69" s="11">
         <v>1</v>
@@ -15276,7 +15323,7 @@
         <v>234</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I70" s="11">
         <v>1</v>
@@ -15343,13 +15390,13 @@
         <v>10</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="I71" s="11">
         <v>5</v>
@@ -15422,7 +15469,7 @@
         <v>234</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I72" s="11">
         <v>1</v>
@@ -15509,7 +15556,7 @@
         <v>234</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="I73" s="11">
         <v>4</v>
@@ -15584,7 +15631,7 @@
         <v>234</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I74" s="13">
         <v>1</v>
@@ -15665,7 +15712,7 @@
         <v>234</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I75" s="13">
         <v>4</v>
@@ -15736,7 +15783,7 @@
         <v>234</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I76" s="11">
         <v>1</v>
@@ -15821,13 +15868,13 @@
         <v>10</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>265</v>
+        <v>327</v>
       </c>
       <c r="G77" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I77" s="11">
         <v>2</v>
@@ -15894,13 +15941,13 @@
         <v>10</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>266</v>
+        <v>328</v>
       </c>
       <c r="G78" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I78" s="11">
         <v>4</v>
@@ -15967,13 +16014,13 @@
         <v>10</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G79" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I79" s="11">
         <v>2</v>
@@ -16046,7 +16093,7 @@
         <v>234</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I80" s="11">
         <v>11</v>
@@ -16119,7 +16166,7 @@
         <v>234</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I81" s="11">
         <v>4</v>
@@ -16190,7 +16237,7 @@
         <v>234</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I82" s="11">
         <v>4</v>
@@ -16261,7 +16308,7 @@
         <v>234</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I83" s="11">
         <v>1</v>
@@ -16352,7 +16399,7 @@
         <v>234</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I84" s="11">
         <v>3</v>
@@ -16427,7 +16474,7 @@
         <v>234</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I85" s="11">
         <v>6</v>
@@ -16492,13 +16539,13 @@
         <v>10</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="G86" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I86" s="11">
         <v>4</v>
@@ -16563,13 +16610,13 @@
         <v>10</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="G87" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I87" s="11">
         <v>2</v>
@@ -16640,7 +16687,7 @@
         <v>234</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I88" s="11">
         <v>6</v>
@@ -16713,7 +16760,7 @@
         <v>234</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I89" s="11">
         <v>2</v>
@@ -16786,7 +16833,7 @@
         <v>234</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I90" s="11">
         <v>11</v>
@@ -16859,7 +16906,7 @@
         <v>234</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I91" s="11">
         <v>11</v>
@@ -16926,13 +16973,13 @@
         <v>10</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I92" s="11">
         <v>11</v>
@@ -17005,7 +17052,7 @@
         <v>234</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I93" s="11">
         <v>6</v>
@@ -17070,13 +17117,13 @@
         <v>10</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I94" s="11">
         <v>2</v>
@@ -17141,13 +17188,13 @@
         <v>10</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I95" s="11">
         <v>4</v>
@@ -17217,10 +17264,10 @@
         <v>235</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="I96" s="11">
         <v>1</v>
@@ -17322,7 +17369,9 @@
       <c r="B97" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C97" s="12"/>
+      <c r="C97" s="12" t="s">
+        <v>125</v>
+      </c>
       <c r="D97" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
@@ -17332,13 +17381,13 @@
         <v>30</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G97" s="11" t="s">
         <v>225</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I97" s="11">
         <v>1</v>
@@ -17409,13 +17458,13 @@
         <v>30</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>287</v>
+        <v>333</v>
       </c>
       <c r="G98" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I98" s="13">
         <v>1</v>
@@ -17484,13 +17533,13 @@
         <v>30</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G99" s="11" t="s">
         <v>225</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I99" s="11">
         <v>11</v>
@@ -17557,13 +17606,13 @@
         <v>30</v>
       </c>
       <c r="F100" s="11" t="s">
-        <v>286</v>
+        <v>334</v>
       </c>
       <c r="G100" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I100" s="11">
         <v>11</v>
@@ -17638,7 +17687,7 @@
         <v>234</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I101" s="11">
         <v>6</v>
@@ -17711,7 +17760,7 @@
         <v>234</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I102" s="11">
         <v>1</v>
@@ -17812,7 +17861,7 @@
         <v>234</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I103" s="11">
         <v>4</v>
@@ -17883,7 +17932,7 @@
         <v>234</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I104" s="11">
         <v>3</v>
@@ -17948,13 +17997,13 @@
         <v>10</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="I105" s="11">
         <v>3</v>
@@ -18005,7 +18054,7 @@
         <v>66</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C106" s="11" t="s">
         <v>124</v>
@@ -18019,13 +18068,13 @@
         <v>10</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H106" s="11" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="I106" s="11">
         <v>2</v>
@@ -18078,7 +18127,7 @@
         <v>66</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C107" s="11" t="s">
         <v>5</v>
@@ -18098,7 +18147,7 @@
         <v>234</v>
       </c>
       <c r="H107" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I107" s="11">
         <v>4</v>
@@ -18169,7 +18218,7 @@
         <v>234</v>
       </c>
       <c r="H108" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I108" s="11">
         <v>1</v>
@@ -18260,7 +18309,7 @@
         <v>234</v>
       </c>
       <c r="H109" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I109" s="11">
         <v>6</v>
@@ -18327,13 +18376,13 @@
         <v>10</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>259</v>
+        <v>336</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H110" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I110" s="11">
         <v>1</v>
@@ -18414,13 +18463,13 @@
         <v>10</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I111" s="11">
         <v>4</v>
@@ -18491,7 +18540,7 @@
         <v>234</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I112" s="11">
         <v>4</v>
@@ -18558,13 +18607,13 @@
         <v>10</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>259</v>
+        <v>337</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H113" s="11" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="I113" s="11">
         <v>1</v>
@@ -18655,7 +18704,7 @@
         <v>234</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I114" s="11">
         <v>2</v>
@@ -18732,7 +18781,7 @@
         <v>234</v>
       </c>
       <c r="H115" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I115" s="11">
         <v>3</v>
@@ -18803,7 +18852,7 @@
         <v>234</v>
       </c>
       <c r="H116" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I116" s="11">
         <v>4</v>
@@ -18876,7 +18925,7 @@
         <v>234</v>
       </c>
       <c r="H117" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I117" s="11">
         <v>1</v>
@@ -18967,7 +19016,7 @@
         <v>234</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I118" s="11">
         <v>3</v>
@@ -19032,13 +19081,13 @@
         <v>10</v>
       </c>
       <c r="F119" s="12" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>317</v>
+        <v>338</v>
       </c>
       <c r="I119" s="11">
         <v>2</v>
@@ -19111,7 +19160,7 @@
         <v>234</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I120" s="11">
         <v>1</v>
@@ -19196,13 +19245,13 @@
         <v>10</v>
       </c>
       <c r="F121" s="12" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H121" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I121" s="11">
         <v>3</v>
@@ -19273,7 +19322,7 @@
         <v>234</v>
       </c>
       <c r="H122" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I122" s="11">
         <v>3</v>
@@ -19338,13 +19387,13 @@
         <v>10</v>
       </c>
       <c r="F123" s="12" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H123" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I123" s="11">
         <v>1</v>
@@ -19408,12 +19457,14 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F124" s="12"/>
+      <c r="F124" s="12" t="s">
+        <v>259</v>
+      </c>
       <c r="G124" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H124" s="11" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I124" s="11">
         <v>1</v>
@@ -19497,12 +19548,14 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F125" s="12"/>
+      <c r="F125" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="G125" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H125" s="11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="I125" s="11">
         <v>4</v>
@@ -19575,7 +19628,7 @@
         <v>234</v>
       </c>
       <c r="H126" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I126" s="11">
         <v>1</v>
@@ -19659,12 +19712,14 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F127" s="12"/>
+      <c r="F127" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="G127" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H127" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I127" s="11">
         <v>4</v>
@@ -19737,7 +19792,7 @@
         <v>234</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I128" s="11">
         <v>3</v>
@@ -19804,13 +19859,13 @@
         <v>10</v>
       </c>
       <c r="F129" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H129" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I129" s="11">
         <v>1</v>
@@ -19874,12 +19929,14 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F130" s="12"/>
+      <c r="F130" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="G130" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H130" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I130" s="11">
         <v>3</v>
@@ -19951,10 +20008,10 @@
         <v>236</v>
       </c>
       <c r="G131" s="11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H131" s="11" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="I131" s="11">
         <v>1</v>
@@ -20068,13 +20125,13 @@
         <v>60</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G132" s="11" t="s">
         <v>225</v>
       </c>
       <c r="H132" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I132" s="11">
         <v>1</v>
@@ -20145,13 +20202,13 @@
         <v>60</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="G133" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H133" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I133" s="11">
         <v>1</v>
@@ -20226,7 +20283,7 @@
         <v>234</v>
       </c>
       <c r="H134" s="11" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="I134" s="11">
         <v>1</v>
@@ -20293,13 +20350,13 @@
         <v>60</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G135" s="11" t="s">
         <v>225</v>
       </c>
       <c r="H135" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I135" s="11">
         <v>11</v>
@@ -20366,13 +20423,13 @@
         <v>60</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
       <c r="G136" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H136" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I136" s="11">
         <v>11</v>
@@ -20441,13 +20498,13 @@
         <v>60</v>
       </c>
       <c r="F137" s="11" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="G137" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H137" s="11" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I137" s="11">
         <v>1</v>
@@ -20503,7 +20560,7 @@
         <v>23</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="D138" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -20514,13 +20571,13 @@
         <v>60</v>
       </c>
       <c r="F138" s="37" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="G138" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H138" s="11" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I138" s="11">
         <v>1</v>
@@ -20593,7 +20650,7 @@
         <v>234</v>
       </c>
       <c r="H139" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I139" s="11">
         <v>1</v>
@@ -20679,13 +20736,13 @@
         <v>10</v>
       </c>
       <c r="F140" s="11" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G140" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H140" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I140" s="11">
         <v>2</v>
@@ -20750,13 +20807,13 @@
         <v>10</v>
       </c>
       <c r="F141" s="11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G141" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H141" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I141" s="11">
         <v>4</v>
@@ -20821,13 +20878,13 @@
         <v>10</v>
       </c>
       <c r="F142" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G142" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H142" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I142" s="11">
         <v>3</v>
@@ -20898,7 +20955,7 @@
         <v>234</v>
       </c>
       <c r="H143" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I143" s="11">
         <v>5</v>
@@ -20969,7 +21026,7 @@
         <v>234</v>
       </c>
       <c r="H144" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I144" s="11">
         <v>2</v>
@@ -21038,7 +21095,7 @@
         <v>234</v>
       </c>
       <c r="H145" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I145" s="11">
         <v>4</v>
@@ -21107,7 +21164,7 @@
         <v>234</v>
       </c>
       <c r="H146" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I146" s="11">
         <v>3</v>
@@ -21176,7 +21233,7 @@
         <v>234</v>
       </c>
       <c r="H147" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I147" s="11">
         <v>6</v>
@@ -21245,7 +21302,7 @@
         <v>234</v>
       </c>
       <c r="H148" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I148" s="11">
         <v>6</v>
@@ -21314,7 +21371,7 @@
         <v>234</v>
       </c>
       <c r="H149" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I149" s="11">
         <v>3</v>
@@ -21383,7 +21440,7 @@
         <v>234</v>
       </c>
       <c r="H150" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I150" s="11">
         <v>7</v>
@@ -21452,7 +21509,7 @@
         <v>234</v>
       </c>
       <c r="H151" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I151" s="11">
         <v>11</v>
@@ -21521,7 +21578,7 @@
         <v>234</v>
       </c>
       <c r="H152" s="11" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="I152" s="11">
         <v>6</v>
@@ -21569,10 +21626,10 @@
     </row>
     <row r="153" spans="1:38">
       <c r="A153" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B153" s="28" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C153" s="11" t="s">
         <v>5</v>
@@ -21586,13 +21643,13 @@
         <v>10</v>
       </c>
       <c r="F153" s="11" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="G153" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H153" s="11" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="I153" s="11">
         <v>4</v>
@@ -21640,10 +21697,10 @@
     </row>
     <row r="154" spans="1:38">
       <c r="A154" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B154" s="28" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C154" s="11" t="s">
         <v>5</v>
@@ -21657,13 +21714,13 @@
         <v>10</v>
       </c>
       <c r="F154" s="11" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="G154" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H154" s="11" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="I154" s="11">
         <v>6</v>
@@ -21711,10 +21768,10 @@
     </row>
     <row r="155" spans="1:38">
       <c r="A155" s="3" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B155" s="28" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C155" s="11" t="s">
         <v>5</v>
@@ -21728,20 +21785,20 @@
         <v>10</v>
       </c>
       <c r="F155" s="11" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G155" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H155" s="11" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="I155" s="11">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="J155" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="K155" s="11"/>
       <c r="L155" s="18"/>
@@ -21759,33 +21816,33 @@
       <c r="X155" s="20"/>
       <c r="Y155" s="20"/>
       <c r="Z155" s="20"/>
-      <c r="AA155" s="20"/>
+      <c r="AA155" s="20">
+        <v>0.2</v>
+      </c>
       <c r="AB155" s="20"/>
       <c r="AC155" s="20"/>
       <c r="AD155" s="20"/>
       <c r="AE155" s="20"/>
       <c r="AF155" s="20"/>
       <c r="AG155" s="20"/>
-      <c r="AH155" s="20">
-        <v>1</v>
-      </c>
+      <c r="AH155" s="20"/>
       <c r="AI155" s="20"/>
       <c r="AJ155" s="20"/>
       <c r="AK155" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="AL155" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:38">
       <c r="A156" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B156" s="28" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="C156" s="11" t="s">
         <v>5</v>
@@ -21796,23 +21853,23 @@
       </c>
       <c r="E156" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F156" s="11" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G156" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H156" s="11" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="I156" s="11">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J156" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K156" s="11"/>
       <c r="L156" s="18"/>
@@ -21837,10 +21894,10 @@
       <c r="AE156" s="20"/>
       <c r="AF156" s="20"/>
       <c r="AG156" s="20"/>
-      <c r="AH156" s="20">
+      <c r="AH156" s="20"/>
+      <c r="AI156" s="20">
         <v>0.5</v>
       </c>
-      <c r="AI156" s="20"/>
       <c r="AJ156" s="20"/>
       <c r="AK156" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
@@ -21848,18 +21905,18 @@
       </c>
       <c r="AL156" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:38">
       <c r="A157" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B157" s="28" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D157" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -21867,23 +21924,23 @@
       </c>
       <c r="E157" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F157" s="11" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G157" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H157" s="11" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="I157" s="11">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="J157" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="K157" s="11"/>
       <c r="L157" s="18"/>
@@ -21908,26 +21965,26 @@
       <c r="AE157" s="20"/>
       <c r="AF157" s="20"/>
       <c r="AG157" s="20"/>
-      <c r="AH157" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="AI157" s="20"/>
+      <c r="AH157" s="20"/>
+      <c r="AI157" s="20">
+        <v>0.3</v>
+      </c>
       <c r="AJ157" s="20"/>
       <c r="AK157" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AL157" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" spans="1:38">
       <c r="A158" s="3" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B158" s="28" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C158" s="11" t="s">
         <v>5</v>
@@ -21941,22 +21998,24 @@
         <v>20</v>
       </c>
       <c r="F158" s="11" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
       <c r="G158" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H158" s="11" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="I158" s="11">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J158" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>40</v>
       </c>
-      <c r="K158" s="11"/>
+      <c r="K158" s="11">
+        <v>20</v>
+      </c>
       <c r="L158" s="18"/>
       <c r="M158" s="18"/>
       <c r="N158" s="18"/>
@@ -21967,9 +22026,7 @@
       <c r="S158" s="19"/>
       <c r="T158" s="18"/>
       <c r="U158" s="18"/>
-      <c r="V158" s="18">
-        <v>0.5</v>
-      </c>
+      <c r="V158" s="18"/>
       <c r="W158" s="19"/>
       <c r="X158" s="20"/>
       <c r="Y158" s="20"/>
@@ -21982,7 +22039,9 @@
       <c r="AF158" s="20"/>
       <c r="AG158" s="20"/>
       <c r="AH158" s="20"/>
-      <c r="AI158" s="20"/>
+      <c r="AI158" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AJ158" s="20"/>
       <c r="AK158" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
@@ -21990,15 +22049,15 @@
       </c>
       <c r="AL158" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:38">
       <c r="A159" s="3" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B159" s="28" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C159" s="11" t="s">
         <v>4</v>
@@ -22012,22 +22071,24 @@
         <v>20</v>
       </c>
       <c r="F159" s="11" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="G159" s="11" t="s">
         <v>234</v>
       </c>
       <c r="H159" s="11" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="I159" s="11">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J159" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>40</v>
       </c>
-      <c r="K159" s="11"/>
+      <c r="K159" s="11">
+        <v>1</v>
+      </c>
       <c r="L159" s="18"/>
       <c r="M159" s="18"/>
       <c r="N159" s="18"/>
@@ -22038,9 +22099,7 @@
       <c r="S159" s="19"/>
       <c r="T159" s="18"/>
       <c r="U159" s="18"/>
-      <c r="V159" s="18">
-        <v>0.5</v>
-      </c>
+      <c r="V159" s="18"/>
       <c r="W159" s="19"/>
       <c r="X159" s="20"/>
       <c r="Y159" s="20"/>
@@ -22048,7 +22107,9 @@
       <c r="AA159" s="20"/>
       <c r="AB159" s="20"/>
       <c r="AC159" s="20"/>
-      <c r="AD159" s="20"/>
+      <c r="AD159" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AE159" s="20"/>
       <c r="AF159" s="20"/>
       <c r="AG159" s="20"/>
@@ -22061,7 +22122,80 @@
       </c>
       <c r="AL159" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:38">
+      <c r="A160" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B160" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="C160" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D160" s="29">
+        <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
+        <v>50</v>
+      </c>
+      <c r="E160" s="29">
+        <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
+        <v>20</v>
+      </c>
+      <c r="F160" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G160" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="H160" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="I160" s="11">
+        <v>2</v>
+      </c>
+      <c r="J160" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>40</v>
+      </c>
+      <c r="K160" s="11">
+        <v>8</v>
+      </c>
+      <c r="L160" s="18"/>
+      <c r="M160" s="18"/>
+      <c r="N160" s="18"/>
+      <c r="O160" s="19"/>
+      <c r="P160" s="18"/>
+      <c r="Q160" s="18"/>
+      <c r="R160" s="18"/>
+      <c r="S160" s="19"/>
+      <c r="T160" s="18"/>
+      <c r="U160" s="18"/>
+      <c r="V160" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="W160" s="19"/>
+      <c r="X160" s="20"/>
+      <c r="Y160" s="20"/>
+      <c r="Z160" s="20"/>
+      <c r="AA160" s="20"/>
+      <c r="AB160" s="20"/>
+      <c r="AC160" s="20"/>
+      <c r="AD160" s="20"/>
+      <c r="AE160" s="20"/>
+      <c r="AF160" s="20"/>
+      <c r="AG160" s="20"/>
+      <c r="AH160" s="20"/>
+      <c r="AI160" s="20"/>
+      <c r="AJ160" s="20"/>
+      <c r="AK160" s="27">
+        <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AL160" s="27">
+        <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -22085,16 +22219,16 @@
       <selection pane="bottomRight" activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" style="10" customWidth="1"/>
-    <col min="7" max="15" width="16.265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17.265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="8.73046875" style="16"/>
+    <col min="6" max="6" width="10.7265625" style="10" customWidth="1"/>
+    <col min="7" max="15" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="17.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -28240,18 +28374,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D548CE7-BEAC-43FA-847F-FDE82E3A5926}">
   <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView topLeftCell="I73" workbookViewId="0">
+      <selection activeCell="U101" sqref="U101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.796875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="5" customWidth="1"/>
   </cols>
@@ -28279,7 +28413,7 @@
         <v>143</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>141</v>
@@ -28294,7 +28428,7 @@
         <v>145</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>199</v>
@@ -28303,16 +28437,16 @@
         <v>200</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>245</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>217</v>
@@ -30711,7 +30845,7 @@
         <v>66</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>137</v>
@@ -32078,7 +32212,7 @@
     </row>
     <row r="74" spans="1:23">
       <c r="A74" s="3" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>257</v>
@@ -33226,10 +33360,10 @@
     </row>
     <row r="96" spans="1:23">
       <c r="A96" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="28" t="s">
@@ -33271,10 +33405,10 @@
     </row>
     <row r="97" spans="1:23">
       <c r="A97" s="3" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="28" t="s">
@@ -33316,10 +33450,10 @@
     </row>
     <row r="98" spans="1:23">
       <c r="A98" s="3" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="28" t="s">
@@ -33361,10 +33495,10 @@
     </row>
     <row r="99" spans="1:23">
       <c r="A99" s="3" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="28" t="s">
@@ -33406,10 +33540,10 @@
     </row>
     <row r="100" spans="1:23">
       <c r="A100" s="3" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="28" t="s">
@@ -33438,15 +33572,15 @@
         <v>4</v>
       </c>
       <c r="U100">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="V100">
         <f>100-Table2[[#This Row],[Exam Weight (%)]]</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="W100">
         <f>IF(COUNTIF(Table1[Module Code],Table2[[#This Row],[Module Code]])&gt;0,SUMIFS(Table1[Sub-total],Table1[Module Code],Table2[[#This Row],[Module Code]],Table1[Summative],"Y")*100,SUMIFS(Table1[Sub-total],Table1[Module Code],Table2[[#This Row],[Alternative Module Code]],Table1[Summative],"Y")*100)</f>
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="101" spans="1:23">
@@ -33674,11 +33808,11 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.59765625" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
adjusted for timetables and MSc deadlines
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1127" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14445E1-5821-47AE-BDAD-E11D19FB04D9}"/>
+  <xr:revisionPtr revIDLastSave="1252" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35134493-AC8E-40D3-B5E8-571F6CF9358D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2811" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="367">
   <si>
     <t>Module Code</t>
   </si>
@@ -1112,13 +1112,37 @@
     <t>Gregynog (*)</t>
   </si>
   <si>
-    <t>Practical Skills</t>
-  </si>
-  <si>
     <t>Lab report</t>
   </si>
   <si>
-    <t>Performance</t>
+    <t>Online test 1</t>
+  </si>
+  <si>
+    <t>Online test 2</t>
+  </si>
+  <si>
+    <t>Reflective Statement</t>
+  </si>
+  <si>
+    <t>Supervisor Assess.</t>
+  </si>
+  <si>
+    <t>Microproject viva (*)</t>
+  </si>
+  <si>
+    <t>Online Training</t>
+  </si>
+  <si>
+    <t>Research paper</t>
+  </si>
+  <si>
+    <t>Project plan</t>
+  </si>
+  <si>
+    <t>Practical Skills (P)</t>
+  </si>
+  <si>
+    <t>Performance (P)</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1367,9 +1391,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1380,9 +1401,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9024,7 +9042,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9473,8 +9491,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}" name="Table1" displayName="Table1" ref="A1:AL167" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102" totalsRowBorderDxfId="101">
-  <autoFilter ref="A1:AL167" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}" name="Table1" displayName="Table1" ref="A1:AL168" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102" totalsRowBorderDxfId="101">
+  <autoFilter ref="A1:AL168" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI141">
     <sortCondition ref="A1:A141"/>
   </sortState>
@@ -9939,13 +9957,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66039B40-29AD-4D93-B125-EAF72A7B3996}">
-  <dimension ref="A1:AL167"/>
+  <dimension ref="A1:AL168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F150" sqref="F150"/>
+      <selection pane="bottomRight" activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15130,14 +15148,14 @@
       <c r="B67" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="51" t="s">
+      <c r="C67" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D67" s="52">
+      <c r="D67" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E67" s="52">
+      <c r="E67" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
@@ -15150,14 +15168,14 @@
       <c r="H67" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="I67" s="51">
+      <c r="I67" s="11">
         <v>1</v>
       </c>
-      <c r="J67" s="53">
+      <c r="J67" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>1</v>
       </c>
-      <c r="K67" s="51">
+      <c r="K67" s="11">
         <v>0.5</v>
       </c>
       <c r="L67" s="18"/>
@@ -15193,11 +15211,11 @@
       <c r="AH67" s="20"/>
       <c r="AI67" s="20"/>
       <c r="AJ67" s="20"/>
-      <c r="AK67" s="54">
+      <c r="AK67" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.1</v>
       </c>
-      <c r="AL67" s="54">
+      <c r="AL67" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>2</v>
       </c>
@@ -15384,7 +15402,9 @@
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>10</v>
       </c>
-      <c r="K70" s="11"/>
+      <c r="K70" s="11">
+        <v>5</v>
+      </c>
       <c r="L70" s="18"/>
       <c r="M70" s="18"/>
       <c r="N70" s="18">
@@ -15422,7 +15442,7 @@
       </c>
       <c r="AL70" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:38">
@@ -15657,14 +15677,14 @@
       <c r="B74" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C74" s="51" t="s">
+      <c r="C74" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D74" s="52">
+      <c r="D74" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E74" s="52">
+      <c r="E74" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
@@ -15677,14 +15697,14 @@
       <c r="H74" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I74" s="51">
+      <c r="I74" s="11">
         <v>1</v>
       </c>
-      <c r="J74" s="53">
+      <c r="J74" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>1</v>
       </c>
-      <c r="K74" s="51">
+      <c r="K74" s="11">
         <v>0.5</v>
       </c>
       <c r="L74" s="18"/>
@@ -15720,11 +15740,11 @@
       <c r="AH74" s="20"/>
       <c r="AI74" s="20"/>
       <c r="AJ74" s="20"/>
-      <c r="AK74" s="54">
+      <c r="AK74" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.1</v>
       </c>
-      <c r="AL74" s="54">
+      <c r="AL74" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>2</v>
       </c>
@@ -19417,18 +19437,18 @@
       <c r="B123" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C123" s="51" t="s">
+      <c r="C123" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D123" s="52">
+      <c r="D123" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="E123" s="52">
+      <c r="E123" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F123" s="51" t="s">
+      <c r="F123" s="11" t="s">
         <v>351</v>
       </c>
       <c r="G123" s="11" t="s">
@@ -19437,14 +19457,14 @@
       <c r="H123" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I123" s="51">
+      <c r="I123" s="11">
         <v>1</v>
       </c>
-      <c r="J123" s="53">
+      <c r="J123" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>0.8</v>
       </c>
-      <c r="K123" s="51">
+      <c r="K123" s="11">
         <v>0.5</v>
       </c>
       <c r="L123" s="18"/>
@@ -19482,11 +19502,11 @@
       </c>
       <c r="AI123" s="20"/>
       <c r="AJ123" s="20"/>
-      <c r="AK123" s="54">
+      <c r="AK123" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.1</v>
       </c>
-      <c r="AL123" s="54">
+      <c r="AL123" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>2.5</v>
       </c>
@@ -20254,18 +20274,18 @@
       <c r="B134" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C134" s="55" t="s">
+      <c r="C134" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="52">
+      <c r="D134" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E134" s="52">
+      <c r="E134" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F134" s="55" t="s">
+      <c r="F134" s="12" t="s">
         <v>354</v>
       </c>
       <c r="G134" s="11" t="s">
@@ -20274,14 +20294,14 @@
       <c r="H134" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I134" s="51">
+      <c r="I134" s="11">
         <v>3</v>
       </c>
-      <c r="J134" s="53">
+      <c r="J134" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>16</v>
       </c>
-      <c r="K134" s="51"/>
+      <c r="K134" s="11"/>
       <c r="L134" s="18"/>
       <c r="M134" s="18"/>
       <c r="N134" s="18"/>
@@ -20309,11 +20329,11 @@
       <c r="AH134" s="20"/>
       <c r="AI134" s="20"/>
       <c r="AJ134" s="20"/>
-      <c r="AK134" s="54">
+      <c r="AK134" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.4</v>
       </c>
-      <c r="AL134" s="54">
+      <c r="AL134" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>16</v>
       </c>
@@ -20325,18 +20345,18 @@
       <c r="B135" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C135" s="55" t="s">
+      <c r="C135" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D135" s="52">
+      <c r="D135" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E135" s="52">
+      <c r="E135" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F135" s="55" t="s">
+      <c r="F135" s="12" t="s">
         <v>353</v>
       </c>
       <c r="G135" s="11" t="s">
@@ -20345,14 +20365,14 @@
       <c r="H135" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I135" s="51">
+      <c r="I135" s="11">
         <v>3</v>
       </c>
-      <c r="J135" s="53">
+      <c r="J135" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>16</v>
       </c>
-      <c r="K135" s="51"/>
+      <c r="K135" s="11"/>
       <c r="L135" s="18"/>
       <c r="M135" s="18"/>
       <c r="N135" s="18"/>
@@ -20380,11 +20400,11 @@
       </c>
       <c r="AI135" s="20"/>
       <c r="AJ135" s="20"/>
-      <c r="AK135" s="54">
+      <c r="AK135" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.4</v>
       </c>
-      <c r="AL135" s="54">
+      <c r="AL135" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>16</v>
       </c>
@@ -21281,28 +21301,28 @@
       <c r="N147" s="18"/>
       <c r="O147" s="19"/>
       <c r="P147" s="18"/>
-      <c r="Q147" s="18">
-        <v>0.5</v>
-      </c>
+      <c r="Q147" s="18"/>
       <c r="R147" s="18"/>
       <c r="S147" s="19"/>
       <c r="T147" s="18"/>
       <c r="U147" s="18"/>
-      <c r="V147" s="18">
-        <v>0.5</v>
-      </c>
+      <c r="V147" s="18"/>
       <c r="W147" s="19"/>
       <c r="X147" s="20"/>
       <c r="Y147" s="20"/>
       <c r="Z147" s="20"/>
       <c r="AA147" s="20"/>
       <c r="AB147" s="20"/>
-      <c r="AC147" s="20"/>
+      <c r="AC147" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AD147" s="20"/>
       <c r="AE147" s="20"/>
       <c r="AF147" s="20"/>
       <c r="AG147" s="20"/>
-      <c r="AH147" s="20"/>
+      <c r="AH147" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AI147" s="20"/>
       <c r="AJ147" s="20"/>
       <c r="AK147" s="27">
@@ -21315,25 +21335,25 @@
       </c>
     </row>
     <row r="148" spans="1:38">
-      <c r="A148" s="50" t="s">
+      <c r="A148" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C148" s="51" t="s">
+      <c r="C148" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D148" s="52">
+      <c r="D148" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E148" s="52">
+      <c r="E148" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F148" s="51" t="s">
-        <v>356</v>
+      <c r="F148" s="11" t="s">
+        <v>365</v>
       </c>
       <c r="G148" s="11" t="s">
         <v>231</v>
@@ -21341,27 +21361,45 @@
       <c r="H148" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I148" s="51">
-        <v>11</v>
-      </c>
-      <c r="J148" s="53">
+      <c r="I148" s="11">
+        <v>1</v>
+      </c>
+      <c r="J148" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>20</v>
-      </c>
-      <c r="K148" s="51"/>
-      <c r="L148" s="18"/>
-      <c r="M148" s="18"/>
-      <c r="N148" s="18"/>
-      <c r="O148" s="19"/>
-      <c r="P148" s="18"/>
-      <c r="Q148" s="18"/>
-      <c r="R148" s="18"/>
-      <c r="S148" s="19"/>
-      <c r="T148" s="18"/>
-      <c r="U148" s="18"/>
-      <c r="V148" s="18">
-        <v>0.5</v>
-      </c>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="K148" s="11"/>
+      <c r="L148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="M148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="N148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="O148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="P148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="Q148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="R148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="S148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="T148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="U148" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="V148" s="18"/>
       <c r="W148" s="19"/>
       <c r="X148" s="20"/>
       <c r="Y148" s="20"/>
@@ -21376,35 +21414,35 @@
       <c r="AH148" s="20"/>
       <c r="AI148" s="20"/>
       <c r="AJ148" s="20"/>
-      <c r="AK148" s="54">
+      <c r="AK148" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.5</v>
-      </c>
-      <c r="AL148" s="54">
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="AL148" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>20</v>
+        <v>19.999999999999996</v>
       </c>
     </row>
     <row r="149" spans="1:38">
-      <c r="A149" s="50" t="s">
+      <c r="A149" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C149" s="51" t="s">
+      <c r="C149" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D149" s="52">
+      <c r="D149" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E149" s="52">
+      <c r="E149" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F149" s="51" t="s">
-        <v>357</v>
+      <c r="F149" s="11" t="s">
+        <v>366</v>
       </c>
       <c r="G149" s="11" t="s">
         <v>231</v>
@@ -21412,27 +21450,45 @@
       <c r="H149" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I149" s="51">
-        <v>11</v>
-      </c>
-      <c r="J149" s="53">
+      <c r="I149" s="11">
+        <v>1</v>
+      </c>
+      <c r="J149" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>12</v>
-      </c>
-      <c r="K149" s="51"/>
-      <c r="L149" s="18"/>
-      <c r="M149" s="18"/>
-      <c r="N149" s="18"/>
-      <c r="O149" s="19"/>
-      <c r="P149" s="18"/>
-      <c r="Q149" s="18"/>
-      <c r="R149" s="18"/>
-      <c r="S149" s="19"/>
-      <c r="T149" s="18"/>
-      <c r="U149" s="18"/>
-      <c r="V149" s="18">
-        <v>0.3</v>
-      </c>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="K149" s="11"/>
+      <c r="L149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="M149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="N149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="O149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="P149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="Q149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="R149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="S149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="T149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="U149" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="V149" s="18"/>
       <c r="W149" s="19"/>
       <c r="X149" s="20"/>
       <c r="Y149" s="20"/>
@@ -21447,35 +21503,35 @@
       <c r="AH149" s="20"/>
       <c r="AI149" s="20"/>
       <c r="AJ149" s="20"/>
-      <c r="AK149" s="54">
+      <c r="AK149" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.3</v>
-      </c>
-      <c r="AL149" s="54">
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="AL149" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>12</v>
+        <v>7.9999999999999982</v>
       </c>
     </row>
     <row r="150" spans="1:38">
-      <c r="A150" s="50" t="s">
+      <c r="A150" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C150" s="51" t="s">
+      <c r="C150" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D150" s="52">
+      <c r="D150" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E150" s="52">
+      <c r="E150" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F150" s="51" t="s">
-        <v>358</v>
+      <c r="F150" s="11" t="s">
+        <v>356</v>
       </c>
       <c r="G150" s="11" t="s">
         <v>231</v>
@@ -21483,14 +21539,14 @@
       <c r="H150" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I150" s="51">
+      <c r="I150" s="11">
         <v>11</v>
       </c>
-      <c r="J150" s="53">
+      <c r="J150" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>8</v>
-      </c>
-      <c r="K150" s="51"/>
+        <v>12</v>
+      </c>
+      <c r="K150" s="11"/>
       <c r="L150" s="18"/>
       <c r="M150" s="18"/>
       <c r="N150" s="18"/>
@@ -21502,7 +21558,7 @@
       <c r="T150" s="18"/>
       <c r="U150" s="18"/>
       <c r="V150" s="18">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="W150" s="19"/>
       <c r="X150" s="20"/>
@@ -21518,13 +21574,13 @@
       <c r="AH150" s="20"/>
       <c r="AI150" s="20"/>
       <c r="AJ150" s="20"/>
-      <c r="AK150" s="54">
+      <c r="AK150" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.2</v>
-      </c>
-      <c r="AL150" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="AL150" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" spans="1:38">
@@ -21545,7 +21601,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F151" s="11"/>
+      <c r="F151" s="11" t="s">
+        <v>357</v>
+      </c>
       <c r="G151" s="11" t="s">
         <v>231</v>
       </c>
@@ -21557,13 +21615,13 @@
       </c>
       <c r="J151" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K151" s="11"/>
       <c r="L151" s="18"/>
       <c r="M151" s="18"/>
       <c r="N151" s="18">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="O151" s="19"/>
       <c r="P151" s="18"/>
@@ -21589,11 +21647,11 @@
       <c r="AJ151" s="20"/>
       <c r="AK151" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="AL151" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:38">
@@ -21614,7 +21672,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F152" s="11"/>
+      <c r="F152" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="G152" s="11" t="s">
         <v>231</v>
       </c>
@@ -21622,20 +21682,20 @@
         <v>297</v>
       </c>
       <c r="I152" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J152" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="K152" s="11"/>
       <c r="L152" s="18"/>
       <c r="M152" s="18"/>
-      <c r="N152" s="18"/>
+      <c r="N152" s="18">
+        <v>0.05</v>
+      </c>
       <c r="O152" s="19"/>
-      <c r="P152" s="18">
-        <v>0.3</v>
-      </c>
+      <c r="P152" s="18"/>
       <c r="Q152" s="18"/>
       <c r="R152" s="18"/>
       <c r="S152" s="19"/>
@@ -21658,11 +21718,11 @@
       <c r="AJ152" s="20"/>
       <c r="AK152" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="AL152" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:38">
@@ -21683,29 +21743,31 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F153" s="11"/>
+      <c r="F153" s="11" t="s">
+        <v>349</v>
+      </c>
       <c r="G153" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H153" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I153" s="11">
         <v>3</v>
       </c>
       <c r="J153" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="K153" s="11"/>
       <c r="L153" s="18"/>
       <c r="M153" s="18"/>
       <c r="N153" s="18"/>
       <c r="O153" s="19"/>
-      <c r="P153" s="18"/>
-      <c r="Q153" s="18">
-        <v>0.1</v>
-      </c>
+      <c r="P153" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="Q153" s="18"/>
       <c r="R153" s="18"/>
       <c r="S153" s="19"/>
       <c r="T153" s="18"/>
@@ -21727,11 +21789,11 @@
       <c r="AJ153" s="20"/>
       <c r="AK153" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AL153" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:38">
@@ -21752,7 +21814,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F154" s="11"/>
+      <c r="F154" s="11" t="s">
+        <v>359</v>
+      </c>
       <c r="G154" s="11" t="s">
         <v>231</v>
       </c>
@@ -21764,22 +21828,24 @@
       </c>
       <c r="J154" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>24</v>
-      </c>
-      <c r="K154" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="K154" s="11">
+        <v>4</v>
+      </c>
       <c r="L154" s="18"/>
       <c r="M154" s="18"/>
       <c r="N154" s="18"/>
       <c r="O154" s="19"/>
       <c r="P154" s="18"/>
-      <c r="Q154" s="18"/>
+      <c r="Q154" s="18">
+        <v>0.1</v>
+      </c>
       <c r="R154" s="18"/>
       <c r="S154" s="19"/>
       <c r="T154" s="18"/>
       <c r="U154" s="18"/>
-      <c r="V154" s="18">
-        <v>0.3</v>
-      </c>
+      <c r="V154" s="18"/>
       <c r="W154" s="19"/>
       <c r="X154" s="20"/>
       <c r="Y154" s="20"/>
@@ -21796,11 +21862,11 @@
       <c r="AJ154" s="20"/>
       <c r="AK154" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="AL154" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:38">
@@ -21821,7 +21887,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F155" s="11"/>
+      <c r="F155" s="11" t="s">
+        <v>360</v>
+      </c>
       <c r="G155" s="11" t="s">
         <v>231</v>
       </c>
@@ -21833,9 +21901,11 @@
       </c>
       <c r="J155" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>16</v>
-      </c>
-      <c r="K155" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="K155" s="11">
+        <v>0.5</v>
+      </c>
       <c r="L155" s="18"/>
       <c r="M155" s="18"/>
       <c r="N155" s="18"/>
@@ -21847,7 +21917,7 @@
       <c r="T155" s="18"/>
       <c r="U155" s="18"/>
       <c r="V155" s="18">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="W155" s="19"/>
       <c r="X155" s="20"/>
@@ -21865,46 +21935,50 @@
       <c r="AJ155" s="20"/>
       <c r="AK155" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="AL155" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>16</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="156" spans="1:38">
       <c r="A156" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C156" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D156" s="29">
+        <v>187</v>
+      </c>
+      <c r="C156" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="D156" s="51">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E156" s="29">
+      <c r="E156" s="51">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F156" s="11"/>
+      <c r="F156" s="50" t="s">
+        <v>361</v>
+      </c>
       <c r="G156" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H156" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="I156" s="11">
-        <v>3</v>
-      </c>
-      <c r="J156" s="11">
+        <v>310</v>
+      </c>
+      <c r="I156" s="50">
+        <v>1</v>
+      </c>
+      <c r="J156" s="52">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>8</v>
-      </c>
-      <c r="K156" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="K156" s="50">
+        <v>1</v>
+      </c>
       <c r="L156" s="18"/>
       <c r="M156" s="18"/>
       <c r="N156" s="18"/>
@@ -21915,13 +21989,13 @@
       <c r="S156" s="19"/>
       <c r="T156" s="18"/>
       <c r="U156" s="18"/>
-      <c r="V156" s="18"/>
+      <c r="V156" s="18">
+        <v>0.2</v>
+      </c>
       <c r="W156" s="19"/>
       <c r="X156" s="20"/>
       <c r="Y156" s="20"/>
-      <c r="Z156" s="20">
-        <v>0.1</v>
-      </c>
+      <c r="Z156" s="20"/>
       <c r="AA156" s="20"/>
       <c r="AB156" s="20"/>
       <c r="AC156" s="20"/>
@@ -21932,13 +22006,13 @@
       <c r="AH156" s="20"/>
       <c r="AI156" s="20"/>
       <c r="AJ156" s="20"/>
-      <c r="AK156" s="27">
+      <c r="AK156" s="53">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.1</v>
-      </c>
-      <c r="AL156" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="AL156" s="53">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:38">
@@ -21949,7 +22023,7 @@
         <v>188</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="D157" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -21959,7 +22033,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F157" s="11"/>
+      <c r="F157" s="11" t="s">
+        <v>362</v>
+      </c>
       <c r="G157" s="11" t="s">
         <v>231</v>
       </c>
@@ -21967,11 +22043,11 @@
         <v>297</v>
       </c>
       <c r="I157" s="11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J157" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="K157" s="11"/>
       <c r="L157" s="18"/>
@@ -21988,13 +22064,13 @@
       <c r="W157" s="19"/>
       <c r="X157" s="20"/>
       <c r="Y157" s="20"/>
-      <c r="Z157" s="20"/>
+      <c r="Z157" s="20">
+        <v>0.05</v>
+      </c>
       <c r="AA157" s="20"/>
       <c r="AB157" s="20"/>
       <c r="AC157" s="20"/>
-      <c r="AD157" s="20">
-        <v>0.3</v>
-      </c>
+      <c r="AD157" s="20"/>
       <c r="AE157" s="20"/>
       <c r="AF157" s="20"/>
       <c r="AG157" s="20"/>
@@ -22003,11 +22079,11 @@
       <c r="AJ157" s="20"/>
       <c r="AK157" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="AL157" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:38">
@@ -22018,7 +22094,7 @@
         <v>188</v>
       </c>
       <c r="C158" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D158" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -22028,7 +22104,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F158" s="11"/>
+      <c r="F158" s="11" t="s">
+        <v>360</v>
+      </c>
       <c r="G158" s="11" t="s">
         <v>231</v>
       </c>
@@ -22036,13 +22114,15 @@
         <v>297</v>
       </c>
       <c r="I158" s="11">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J158" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>16</v>
       </c>
-      <c r="K158" s="11"/>
+      <c r="K158" s="11">
+        <v>0.5</v>
+      </c>
       <c r="L158" s="18"/>
       <c r="M158" s="18"/>
       <c r="N158" s="18"/>
@@ -22061,13 +22141,13 @@
       <c r="AA158" s="20"/>
       <c r="AB158" s="20"/>
       <c r="AC158" s="20"/>
-      <c r="AD158" s="20"/>
+      <c r="AD158" s="20">
+        <v>0.2</v>
+      </c>
       <c r="AE158" s="20"/>
       <c r="AF158" s="20"/>
       <c r="AG158" s="20"/>
-      <c r="AH158" s="20">
-        <v>0.2</v>
-      </c>
+      <c r="AH158" s="20"/>
       <c r="AI158" s="20"/>
       <c r="AJ158" s="20"/>
       <c r="AK158" s="27">
@@ -22076,7 +22156,7 @@
       </c>
       <c r="AL158" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>16</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="159" spans="1:38">
@@ -22087,7 +22167,7 @@
         <v>188</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D159" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -22097,7 +22177,9 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F159" s="11"/>
+      <c r="F159" s="11" t="s">
+        <v>363</v>
+      </c>
       <c r="G159" s="11" t="s">
         <v>231</v>
       </c>
@@ -22109,7 +22191,7 @@
       </c>
       <c r="J159" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K159" s="11"/>
       <c r="L159" s="18"/>
@@ -22129,58 +22211,58 @@
       <c r="Z159" s="20"/>
       <c r="AA159" s="20"/>
       <c r="AB159" s="20"/>
-      <c r="AC159" s="20"/>
+      <c r="AC159" s="20">
+        <v>0.3</v>
+      </c>
       <c r="AD159" s="20"/>
       <c r="AE159" s="20"/>
       <c r="AF159" s="20"/>
       <c r="AG159" s="20"/>
       <c r="AH159" s="20"/>
-      <c r="AI159" s="20">
-        <v>0.4</v>
-      </c>
+      <c r="AI159" s="20"/>
       <c r="AJ159" s="20"/>
       <c r="AK159" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AL159" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:38">
-      <c r="A160" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="B160" s="28" t="s">
-        <v>276</v>
+      <c r="A160" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="D160" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E160" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F160" s="11" t="s">
-        <v>289</v>
+        <v>364</v>
       </c>
       <c r="G160" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H160" s="11" t="s">
-        <v>336</v>
+        <v>297</v>
       </c>
       <c r="I160" s="11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J160" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="K160" s="11"/>
       <c r="L160" s="18"/>
@@ -22189,9 +22271,7 @@
       <c r="O160" s="19"/>
       <c r="P160" s="18"/>
       <c r="Q160" s="18"/>
-      <c r="R160" s="18">
-        <v>0.1</v>
-      </c>
+      <c r="R160" s="18"/>
       <c r="S160" s="19"/>
       <c r="T160" s="18"/>
       <c r="U160" s="18"/>
@@ -22208,15 +22288,17 @@
       <c r="AF160" s="20"/>
       <c r="AG160" s="20"/>
       <c r="AH160" s="20"/>
-      <c r="AI160" s="20"/>
+      <c r="AI160" s="20">
+        <v>0.45</v>
+      </c>
       <c r="AJ160" s="20"/>
       <c r="AK160" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="AL160" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="161" spans="1:38">
@@ -22238,7 +22320,7 @@
         <v>10</v>
       </c>
       <c r="F161" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G161" s="11" t="s">
         <v>231</v>
@@ -22247,11 +22329,11 @@
         <v>336</v>
       </c>
       <c r="I161" s="11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J161" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K161" s="11"/>
       <c r="L161" s="18"/>
@@ -22260,14 +22342,14 @@
       <c r="O161" s="19"/>
       <c r="P161" s="18"/>
       <c r="Q161" s="18"/>
-      <c r="R161" s="18"/>
+      <c r="R161" s="18">
+        <v>0.1</v>
+      </c>
       <c r="S161" s="19"/>
       <c r="T161" s="18"/>
       <c r="U161" s="18"/>
       <c r="V161" s="18"/>
-      <c r="W161" s="19">
-        <v>0.2</v>
-      </c>
+      <c r="W161" s="19"/>
       <c r="X161" s="20"/>
       <c r="Y161" s="20"/>
       <c r="Z161" s="20"/>
@@ -22283,42 +22365,42 @@
       <c r="AJ161" s="20"/>
       <c r="AK161" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AL161" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" spans="1:38">
       <c r="A162" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B162" s="28" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C162" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D162" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E162" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
       <c r="F162" s="11" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="G162" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H162" s="11" t="s">
-        <v>303</v>
+        <v>336</v>
       </c>
       <c r="I162" s="11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J162" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
@@ -22336,13 +22418,13 @@
       <c r="T162" s="18"/>
       <c r="U162" s="18"/>
       <c r="V162" s="18"/>
-      <c r="W162" s="19"/>
+      <c r="W162" s="19">
+        <v>0.2</v>
+      </c>
       <c r="X162" s="20"/>
       <c r="Y162" s="20"/>
       <c r="Z162" s="20"/>
-      <c r="AA162" s="20">
-        <v>0.2</v>
-      </c>
+      <c r="AA162" s="20"/>
       <c r="AB162" s="20"/>
       <c r="AC162" s="20"/>
       <c r="AD162" s="20"/>
@@ -22380,7 +22462,7 @@
         <v>10</v>
       </c>
       <c r="F163" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G163" s="11" t="s">
         <v>231</v>
@@ -22389,11 +22471,11 @@
         <v>303</v>
       </c>
       <c r="I163" s="11">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J163" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K163" s="11"/>
       <c r="L163" s="18"/>
@@ -22411,7 +22493,9 @@
       <c r="X163" s="20"/>
       <c r="Y163" s="20"/>
       <c r="Z163" s="20"/>
-      <c r="AA163" s="20"/>
+      <c r="AA163" s="20">
+        <v>0.2</v>
+      </c>
       <c r="AB163" s="20"/>
       <c r="AC163" s="20"/>
       <c r="AD163" s="20"/>
@@ -22419,17 +22503,15 @@
       <c r="AF163" s="20"/>
       <c r="AG163" s="20"/>
       <c r="AH163" s="20"/>
-      <c r="AI163" s="20">
-        <v>0.5</v>
-      </c>
+      <c r="AI163" s="20"/>
       <c r="AJ163" s="20"/>
       <c r="AK163" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AL163" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="164" spans="1:38">
@@ -22451,7 +22533,7 @@
         <v>10</v>
       </c>
       <c r="F164" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G164" s="11" t="s">
         <v>231</v>
@@ -22460,11 +22542,11 @@
         <v>303</v>
       </c>
       <c r="I164" s="11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J164" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="K164" s="11"/>
       <c r="L164" s="18"/>
@@ -22491,24 +22573,24 @@
       <c r="AG164" s="20"/>
       <c r="AH164" s="20"/>
       <c r="AI164" s="20">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AJ164" s="20"/>
       <c r="AK164" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AL164" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:38">
       <c r="A165" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B165" s="28" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C165" s="11" t="s">
         <v>5</v>
@@ -22519,10 +22601,10 @@
       </c>
       <c r="E165" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F165" s="11" t="s">
-        <v>337</v>
+        <v>306</v>
       </c>
       <c r="G165" s="11" t="s">
         <v>231</v>
@@ -22531,15 +22613,13 @@
         <v>303</v>
       </c>
       <c r="I165" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J165" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
-        <v>40</v>
-      </c>
-      <c r="K165" s="11">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="K165" s="11"/>
       <c r="L165" s="18"/>
       <c r="M165" s="18"/>
       <c r="N165" s="18"/>
@@ -22564,16 +22644,16 @@
       <c r="AG165" s="20"/>
       <c r="AH165" s="20"/>
       <c r="AI165" s="20">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AJ165" s="20"/>
       <c r="AK165" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AL165" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:38">
@@ -22584,7 +22664,7 @@
         <v>283</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D166" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -22595,23 +22675,23 @@
         <v>20</v>
       </c>
       <c r="F166" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G166" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H166" s="11" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="I166" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J166" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>40</v>
       </c>
       <c r="K166" s="11">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L166" s="18"/>
       <c r="M166" s="18"/>
@@ -22631,14 +22711,14 @@
       <c r="AA166" s="20"/>
       <c r="AB166" s="20"/>
       <c r="AC166" s="20"/>
-      <c r="AD166" s="20">
-        <v>0.5</v>
-      </c>
+      <c r="AD166" s="20"/>
       <c r="AE166" s="20"/>
       <c r="AF166" s="20"/>
       <c r="AG166" s="20"/>
       <c r="AH166" s="20"/>
-      <c r="AI166" s="20"/>
+      <c r="AI166" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AJ166" s="20"/>
       <c r="AK166" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
@@ -22646,45 +22726,45 @@
       </c>
       <c r="AL166" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:38">
       <c r="A167" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B167" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C167" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D167" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E167" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
       <c r="F167" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G167" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H167" s="11" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="I167" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J167" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>40</v>
       </c>
       <c r="K167" s="11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L167" s="18"/>
       <c r="M167" s="18"/>
@@ -22696,9 +22776,7 @@
       <c r="S167" s="19"/>
       <c r="T167" s="18"/>
       <c r="U167" s="18"/>
-      <c r="V167" s="18">
-        <v>0.5</v>
-      </c>
+      <c r="V167" s="18"/>
       <c r="W167" s="19"/>
       <c r="X167" s="20"/>
       <c r="Y167" s="20"/>
@@ -22706,7 +22784,9 @@
       <c r="AA167" s="20"/>
       <c r="AB167" s="20"/>
       <c r="AC167" s="20"/>
-      <c r="AD167" s="20"/>
+      <c r="AD167" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AE167" s="20"/>
       <c r="AF167" s="20"/>
       <c r="AG167" s="20"/>
@@ -22718,6 +22798,79 @@
         <v>0.5</v>
       </c>
       <c r="AL167" s="27">
+        <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:38">
+      <c r="A168" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B168" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D168" s="29">
+        <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
+        <v>50</v>
+      </c>
+      <c r="E168" s="29">
+        <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
+        <v>20</v>
+      </c>
+      <c r="F168" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="H168" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="I168" s="11">
+        <v>2</v>
+      </c>
+      <c r="J168" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
+        <v>40</v>
+      </c>
+      <c r="K168" s="11">
+        <v>8</v>
+      </c>
+      <c r="L168" s="18"/>
+      <c r="M168" s="18"/>
+      <c r="N168" s="18"/>
+      <c r="O168" s="19"/>
+      <c r="P168" s="18"/>
+      <c r="Q168" s="18"/>
+      <c r="R168" s="18"/>
+      <c r="S168" s="19"/>
+      <c r="T168" s="18"/>
+      <c r="U168" s="18"/>
+      <c r="V168" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="W168" s="19"/>
+      <c r="X168" s="20"/>
+      <c r="Y168" s="20"/>
+      <c r="Z168" s="20"/>
+      <c r="AA168" s="20"/>
+      <c r="AB168" s="20"/>
+      <c r="AC168" s="20"/>
+      <c r="AD168" s="20"/>
+      <c r="AE168" s="20"/>
+      <c r="AF168" s="20"/>
+      <c r="AG168" s="20"/>
+      <c r="AH168" s="20"/>
+      <c r="AI168" s="20"/>
+      <c r="AJ168" s="20"/>
+      <c r="AK168" s="27">
+        <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AL168" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>8</v>
       </c>
@@ -22737,10 +22890,10 @@
   <dimension ref="A1:AE141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A63" sqref="A63:XFD63"/>
+      <selection pane="bottomRight" activeCell="X64" sqref="X64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -28656,22 +28809,22 @@
         <v>3</v>
       </c>
       <c r="L63" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M63" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N63" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O63" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P63" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q63" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R63" s="32"/>
       <c r="S63" s="33" t="s">
@@ -28710,7 +28863,7 @@
       <c r="AD63" s="33"/>
       <c r="AE63" s="37">
         <f>SUM(Table14[[#This Row],[Autumn Week 1]:[Spring Week 12]])</f>
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:31">
@@ -28788,24 +28941,24 @@
         <v>4</v>
       </c>
       <c r="Y64" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z64" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA64" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB64" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC64" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD64" s="33"/>
       <c r="AE64" s="37">
         <f>SUM(Table14[[#This Row],[Autumn Week 1]:[Spring Week 12]])</f>
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" customFormat="1"/>
@@ -28898,8 +29051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D548CE7-BEAC-43FA-847F-FDE82E3A5926}">
   <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34266,14 +34419,6 @@
       <formula>NOT(ISERROR(SEARCH("SEM1",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:T121">
-    <cfRule type="containsText" dxfId="1" priority="15" operator="containsText" text="O">
-      <formula>NOT(ISERROR(SEARCH("O",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="16" operator="containsText" text="C">
-      <formula>NOT(ISERROR(SEARCH("C",H2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F2:F121">
     <cfRule type="colorScale" priority="169">
       <colorScale>
@@ -34294,6 +34439,14 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:T121">
+    <cfRule type="containsText" dxfId="1" priority="15" operator="containsText" text="O">
+      <formula>NOT(ISERROR(SEARCH("O",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="16" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35064,7 +35217,7 @@
       </c>
       <c r="C33">
         <f>SUMIF(Table1[Module Code],Sheet2!A33,Table1[Total Hours])</f>
-        <v>45.5</v>
+        <v>30.5</v>
       </c>
       <c r="D33">
         <f>INDEX(Table14[Total],MATCH(Sheet2!A33,Table14[Module Code],0))</f>
@@ -35072,11 +35225,11 @@
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>67.5</v>
+        <v>52.5</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>6.75</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -35904,19 +36057,19 @@
       </c>
       <c r="C68">
         <f>SUMIF(Table1[Module Code],Sheet2!A68,Table1[Total Hours])</f>
-        <v>80</v>
+        <v>37.5</v>
       </c>
       <c r="D68">
         <f>INDEX(Table14[Total],MATCH(Sheet2!A68,Table14[Module Code],0))</f>
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E68">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>76.5</v>
       </c>
       <c r="F68">
         <f t="shared" si="1"/>
-        <v>5.65</v>
+        <v>3.8250000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -35928,19 +36081,19 @@
       </c>
       <c r="C69">
         <f>SUMIF(Table1[Module Code],Sheet2!A69,Table1[Total Hours])</f>
-        <v>80</v>
+        <v>64.5</v>
       </c>
       <c r="D69">
         <f>INDEX(Table14[Total],MATCH(Sheet2!A69,Table14[Module Code],0))</f>
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E69">
         <f t="shared" ref="E69" si="2">SUM(C69:D69)</f>
-        <v>124</v>
+        <v>103.5</v>
       </c>
       <c r="F69">
         <f t="shared" ref="F69:F70" si="3">E69/B69</f>
-        <v>6.2</v>
+        <v>5.1749999999999998</v>
       </c>
     </row>
     <row r="70" spans="1:6">

</xml_diff>

<commit_message>
deadlines and workload split by colour
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1444" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B177C1E-3597-454F-889E-74E955895744}"/>
+  <xr:revisionPtr revIDLastSave="1449" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6624DEAD-B975-46D5-9197-10F2020A97B4}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="4560" windowWidth="28800" windowHeight="15370" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="376">
   <si>
     <t>Module Code</t>
   </si>
@@ -1146,9 +1146,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>:B</t>
   </si>
   <si>
     <t>Weekly tests</t>
@@ -1279,7 +1276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1418,24 +1415,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -9078,7 +9057,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9996,10 +9975,10 @@
   <dimension ref="A1:AL174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
+      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13710,7 +13689,7 @@
         <v>20</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>231</v>
@@ -14841,24 +14820,24 @@
       </c>
     </row>
     <row r="63" spans="1:38">
-      <c r="A63" s="54" t="s">
+      <c r="A63" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="55" t="s">
+      <c r="C63" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D63" s="51">
+      <c r="D63" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="E63" s="51">
+      <c r="E63" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F63" s="55" t="s">
+      <c r="F63" s="12" t="s">
         <v>365</v>
       </c>
       <c r="G63" s="11" t="s">
@@ -14867,14 +14846,14 @@
       <c r="H63" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="I63" s="50">
+      <c r="I63" s="11">
         <v>1</v>
       </c>
-      <c r="J63" s="52">
+      <c r="J63" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>0.79999999999999982</v>
       </c>
-      <c r="K63" s="50">
+      <c r="K63" s="11">
         <v>0.5</v>
       </c>
       <c r="L63" s="18">
@@ -14922,11 +14901,11 @@
       <c r="AH63" s="20"/>
       <c r="AI63" s="20"/>
       <c r="AJ63" s="20"/>
-      <c r="AK63" s="53">
+      <c r="AK63" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0</v>
       </c>
-      <c r="AL63" s="53">
+      <c r="AL63" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>5</v>
       </c>
@@ -15180,19 +15159,19 @@
       <c r="B67" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="50" t="s">
-        <v>368</v>
-      </c>
-      <c r="D67" s="51">
+      <c r="C67" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E67" s="51">
+      <c r="E67" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F67" s="50" t="s">
-        <v>369</v>
+      <c r="F67" s="11" t="s">
+        <v>368</v>
       </c>
       <c r="G67" s="11" t="s">
         <v>222</v>
@@ -15200,14 +15179,14 @@
       <c r="H67" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="I67" s="50">
+      <c r="I67" s="11">
         <v>1</v>
       </c>
-      <c r="J67" s="52">
+      <c r="J67" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K67" s="50">
+      <c r="K67" s="11">
         <v>0.5</v>
       </c>
       <c r="L67" s="18"/>
@@ -15251,11 +15230,11 @@
       <c r="AH67" s="20"/>
       <c r="AI67" s="20"/>
       <c r="AJ67" s="20"/>
-      <c r="AK67" s="53">
+      <c r="AK67" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0</v>
       </c>
-      <c r="AL67" s="53">
+      <c r="AL67" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>4</v>
       </c>
@@ -15278,8 +15257,8 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F68" s="50" t="s">
-        <v>370</v>
+      <c r="F68" s="11" t="s">
+        <v>369</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>231</v>
@@ -15351,8 +15330,8 @@
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F69" s="50" t="s">
-        <v>371</v>
+      <c r="F69" s="11" t="s">
+        <v>370</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>231</v>
@@ -15484,18 +15463,18 @@
       <c r="B71" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="50" t="s">
+      <c r="C71" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="51">
+      <c r="D71" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E71" s="51">
+      <c r="E71" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F71" s="50" t="s">
+      <c r="F71" s="11" t="s">
         <v>290</v>
       </c>
       <c r="G71" s="11" t="s">
@@ -15504,14 +15483,14 @@
       <c r="H71" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="I71" s="50">
+      <c r="I71" s="11">
         <v>4</v>
       </c>
-      <c r="J71" s="52">
+      <c r="J71" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>18</v>
       </c>
-      <c r="K71" s="50"/>
+      <c r="K71" s="11"/>
       <c r="L71" s="18"/>
       <c r="M71" s="18"/>
       <c r="N71" s="18"/>
@@ -15539,11 +15518,11 @@
       <c r="AH71" s="20"/>
       <c r="AI71" s="20"/>
       <c r="AJ71" s="20"/>
-      <c r="AK71" s="53">
+      <c r="AK71" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.45</v>
       </c>
-      <c r="AL71" s="53">
+      <c r="AL71" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>18</v>
       </c>
@@ -15851,18 +15830,18 @@
       <c r="B76" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C76" s="50" t="s">
+      <c r="C76" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D76" s="51">
+      <c r="D76" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E76" s="51">
+      <c r="E76" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F76" s="50" t="s">
+      <c r="F76" s="11" t="s">
         <v>365</v>
       </c>
       <c r="G76" s="11" t="s">
@@ -15871,14 +15850,14 @@
       <c r="H76" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="I76" s="50">
+      <c r="I76" s="11">
         <v>1</v>
       </c>
-      <c r="J76" s="52">
+      <c r="J76" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>2.125</v>
       </c>
-      <c r="K76" s="50">
+      <c r="K76" s="11">
         <v>0.5</v>
       </c>
       <c r="L76" s="18">
@@ -15922,11 +15901,11 @@
       <c r="AH76" s="20"/>
       <c r="AI76" s="20"/>
       <c r="AJ76" s="20"/>
-      <c r="AK76" s="53">
+      <c r="AK76" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0</v>
       </c>
-      <c r="AL76" s="53">
+      <c r="AL76" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>4</v>
       </c>
@@ -15938,19 +15917,19 @@
       <c r="B77" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C77" s="50" t="s">
+      <c r="C77" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D77" s="51">
+      <c r="D77" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E77" s="51">
+      <c r="E77" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F77" s="50" t="s">
-        <v>372</v>
+      <c r="F77" s="11" t="s">
+        <v>371</v>
       </c>
       <c r="G77" s="11" t="s">
         <v>231</v>
@@ -15958,14 +15937,14 @@
       <c r="H77" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="I77" s="50">
+      <c r="I77" s="11">
         <v>5</v>
       </c>
-      <c r="J77" s="52">
+      <c r="J77" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>4</v>
       </c>
-      <c r="K77" s="50">
+      <c r="K77" s="11">
         <v>0.5</v>
       </c>
       <c r="L77" s="18"/>
@@ -15995,11 +15974,11 @@
       <c r="AH77" s="20"/>
       <c r="AI77" s="20"/>
       <c r="AJ77" s="20"/>
-      <c r="AK77" s="53">
+      <c r="AK77" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.1</v>
       </c>
-      <c r="AL77" s="53">
+      <c r="AL77" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>0.5</v>
       </c>
@@ -16011,19 +15990,19 @@
       <c r="B78" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C78" s="50" t="s">
+      <c r="C78" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D78" s="51">
+      <c r="D78" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E78" s="51">
+      <c r="E78" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F78" s="50" t="s">
-        <v>373</v>
+      <c r="F78" s="11" t="s">
+        <v>372</v>
       </c>
       <c r="G78" s="11" t="s">
         <v>231</v>
@@ -16031,14 +16010,14 @@
       <c r="H78" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I78" s="50">
+      <c r="I78" s="11">
         <v>5</v>
       </c>
-      <c r="J78" s="52">
+      <c r="J78" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>4</v>
       </c>
-      <c r="K78" s="50">
+      <c r="K78" s="11">
         <v>0.5</v>
       </c>
       <c r="L78" s="18"/>
@@ -16068,11 +16047,11 @@
       <c r="AH78" s="20"/>
       <c r="AI78" s="20"/>
       <c r="AJ78" s="20"/>
-      <c r="AK78" s="53">
+      <c r="AK78" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.1</v>
       </c>
-      <c r="AL78" s="53">
+      <c r="AL78" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>0.5</v>
       </c>
@@ -16084,18 +16063,18 @@
       <c r="B79" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C79" s="50" t="s">
+      <c r="C79" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D79" s="51">
+      <c r="D79" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>100</v>
       </c>
-      <c r="E79" s="51">
+      <c r="E79" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>10</v>
       </c>
-      <c r="F79" s="50" t="s">
+      <c r="F79" s="11" t="s">
         <v>289</v>
       </c>
       <c r="G79" s="11" t="s">
@@ -16104,14 +16083,14 @@
       <c r="H79" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="I79" s="50">
+      <c r="I79" s="11">
         <v>4</v>
       </c>
-      <c r="J79" s="52">
+      <c r="J79" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>14</v>
       </c>
-      <c r="K79" s="50"/>
+      <c r="K79" s="11"/>
       <c r="L79" s="18"/>
       <c r="M79" s="18"/>
       <c r="N79" s="18"/>
@@ -16139,11 +16118,11 @@
       <c r="AH79" s="20"/>
       <c r="AI79" s="20"/>
       <c r="AJ79" s="20"/>
-      <c r="AK79" s="53">
+      <c r="AK79" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>0.35</v>
       </c>
-      <c r="AL79" s="53">
+      <c r="AL79" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>14</v>
       </c>
@@ -16915,7 +16894,7 @@
         <v>20</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>222</v>
@@ -16994,19 +16973,19 @@
       <c r="B91" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C91" s="50" t="s">
+      <c r="C91" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D91" s="51">
+      <c r="D91" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>30</v>
       </c>
-      <c r="E91" s="51">
+      <c r="E91" s="29">
         <f>INDEX(Table2[Credits],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
         <v>20</v>
       </c>
-      <c r="F91" s="50" t="s">
-        <v>374</v>
+      <c r="F91" s="11" t="s">
+        <v>373</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>231</v>
@@ -17014,14 +16993,14 @@
       <c r="H91" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I91" s="50">
+      <c r="I91" s="11">
         <v>11</v>
       </c>
-      <c r="J91" s="52">
+      <c r="J91" s="11">
         <f>AVERAGE(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]])*4*Table1[[#This Row],[Credits]]</f>
         <v>5.6000000000000005</v>
       </c>
-      <c r="K91" s="50"/>
+      <c r="K91" s="11"/>
       <c r="L91" s="18"/>
       <c r="M91" s="18"/>
       <c r="N91" s="18"/>
@@ -17049,11 +17028,11 @@
       </c>
       <c r="AI91" s="20"/>
       <c r="AJ91" s="20"/>
-      <c r="AK91" s="53">
+      <c r="AK91" s="27">
         <f>IF(Table1[[#This Row],[Summative]]="Y",SUMIF(Table1[[#This Row],[Autumn Week 1]:[Spring Exams]],"&gt;0",Table1[[#This Row],[Autumn Week 1]:[Spring Exams]]),0)</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AL91" s="53">
+      <c r="AL91" s="27">
         <f>IF(Table1[[#This Row],[Hours]]&gt;0,Table1[[#This Row],[Hours]],Table1[[#This Row],[Nominal Hours]])*COUNTIF(Table1[[#This Row],[Autumn Week 1]:[Spring Week 12]],"&gt;0")</f>
         <v>5.6000000000000005</v>
       </c>

</xml_diff>

<commit_message>
project work classed as project (not lab)
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1449" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6624DEAD-B975-46D5-9197-10F2020A97B4}"/>
+  <xr:revisionPtr revIDLastSave="1456" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F0B2FFB-31C4-44AA-A778-9A8AC9EBCF19}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -9057,7 +9057,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9507,7 +9507,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}" name="Table1" displayName="Table1" ref="A1:AL174" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102" totalsRowBorderDxfId="101">
-  <autoFilter ref="A1:AL174" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}"/>
+  <autoFilter ref="A1:AL174" xr:uid="{FA69A777-C149-48BD-B248-35F32F0AC920}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="LB"/>
+        <filter val="PJ"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI147">
     <sortCondition ref="A1:A147"/>
   </sortState>
@@ -9975,10 +9982,10 @@
   <dimension ref="A1:AL174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomRight" activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10111,7 +10118,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" hidden="1">
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
@@ -10190,7 +10197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" hidden="1">
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
@@ -10263,7 +10270,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" hidden="1">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -10336,7 +10343,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" hidden="1">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -10427,7 +10434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" hidden="1">
       <c r="A6" s="4" t="s">
         <v>60</v>
       </c>
@@ -10504,7 +10511,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" hidden="1">
       <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
@@ -10575,7 +10582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" hidden="1">
       <c r="A8" s="4" t="s">
         <v>60</v>
       </c>
@@ -10802,7 +10809,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" hidden="1">
       <c r="A11" s="4" t="s">
         <v>62</v>
       </c>
@@ -10875,7 +10882,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" hidden="1">
       <c r="A12" s="3" t="s">
         <v>84</v>
       </c>
@@ -11057,7 +11064,7 @@
         <v>19.999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" hidden="1">
       <c r="A14" s="3" t="s">
         <v>190</v>
       </c>
@@ -11130,7 +11137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" hidden="1">
       <c r="A15" s="3" t="s">
         <v>190</v>
       </c>
@@ -11205,7 +11212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" hidden="1">
       <c r="A16" s="3" t="s">
         <v>86</v>
       </c>
@@ -11286,7 +11293,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" hidden="1">
       <c r="A17" s="3" t="s">
         <v>86</v>
       </c>
@@ -11357,7 +11364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" hidden="1">
       <c r="A18" s="3" t="s">
         <v>86</v>
       </c>
@@ -11430,7 +11437,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" hidden="1">
       <c r="A19" s="3" t="s">
         <v>87</v>
       </c>
@@ -11507,7 +11514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" hidden="1">
       <c r="A20" s="3" t="s">
         <v>85</v>
       </c>
@@ -11578,7 +11585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" hidden="1">
       <c r="A21" s="3" t="s">
         <v>85</v>
       </c>
@@ -11649,7 +11656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" hidden="1">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -11740,7 +11747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" hidden="1">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -11815,7 +11822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" hidden="1">
       <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
@@ -11913,7 +11920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" hidden="1">
       <c r="A25" s="4" t="s">
         <v>47</v>
       </c>
@@ -11986,7 +11993,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" hidden="1">
       <c r="A26" s="4" t="s">
         <v>235</v>
       </c>
@@ -12077,7 +12084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" hidden="1">
       <c r="A27" s="4" t="s">
         <v>235</v>
       </c>
@@ -12154,7 +12161,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" hidden="1">
       <c r="A28" s="4" t="s">
         <v>235</v>
       </c>
@@ -12227,7 +12234,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" hidden="1">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
@@ -12375,7 +12382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" hidden="1">
       <c r="A31" s="4" t="s">
         <v>50</v>
       </c>
@@ -12448,7 +12455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" hidden="1">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
@@ -12521,7 +12528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" hidden="1">
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
@@ -12600,7 +12607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" hidden="1">
       <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
@@ -12691,7 +12698,7 @@
         <v>2.0000000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:38" hidden="1">
       <c r="A35" s="4" t="s">
         <v>45</v>
       </c>
@@ -12768,7 +12775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" hidden="1">
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
@@ -12843,7 +12850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:38" hidden="1">
       <c r="A37" s="4" t="s">
         <v>45</v>
       </c>
@@ -12997,7 +13004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" hidden="1">
       <c r="A39" s="4" t="s">
         <v>46</v>
       </c>
@@ -13068,7 +13075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" hidden="1">
       <c r="A40" s="4" t="s">
         <v>52</v>
       </c>
@@ -13301,7 +13308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" hidden="1">
       <c r="A43" s="4" t="s">
         <v>52</v>
       </c>
@@ -13374,7 +13381,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:38" hidden="1">
       <c r="A44" s="4" t="s">
         <v>52</v>
       </c>
@@ -13526,7 +13533,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:38" hidden="1">
       <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
@@ -13597,7 +13604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:38" hidden="1">
       <c r="A47" s="4" t="s">
         <v>54</v>
       </c>
@@ -13670,7 +13677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:38" hidden="1">
       <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
@@ -13741,7 +13748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" hidden="1">
       <c r="A49" s="3" t="s">
         <v>96</v>
       </c>
@@ -13832,7 +13839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" hidden="1">
       <c r="A50" s="3" t="s">
         <v>96</v>
       </c>
@@ -13907,7 +13914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" hidden="1">
       <c r="A51" s="3" t="s">
         <v>97</v>
       </c>
@@ -13915,7 +13922,7 @@
         <v>89</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="D51" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -13982,7 +13989,7 @@
         <v>12.000000000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" hidden="1">
       <c r="A52" s="3" t="s">
         <v>189</v>
       </c>
@@ -14073,7 +14080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" hidden="1">
       <c r="A53" s="3" t="s">
         <v>92</v>
       </c>
@@ -14144,7 +14151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" hidden="1">
       <c r="A54" s="3" t="s">
         <v>92</v>
       </c>
@@ -14302,7 +14309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" hidden="1">
       <c r="A56" s="3" t="s">
         <v>94</v>
       </c>
@@ -14373,7 +14380,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="57" spans="1:38" ht="14.65" customHeight="1">
+    <row r="57" spans="1:38" ht="14.65" hidden="1" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>94</v>
       </c>
@@ -14446,7 +14453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:38" hidden="1">
       <c r="A58" s="3" t="s">
         <v>94</v>
       </c>
@@ -14604,7 +14611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:38" hidden="1">
       <c r="A60" s="3" t="s">
         <v>98</v>
       </c>
@@ -14675,7 +14682,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:38" hidden="1">
       <c r="A61" s="3" t="s">
         <v>98</v>
       </c>
@@ -14748,7 +14755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:38" hidden="1">
       <c r="A62" s="3" t="s">
         <v>98</v>
       </c>
@@ -14819,7 +14826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:38" hidden="1">
       <c r="A63" s="3" t="s">
         <v>1</v>
       </c>
@@ -14910,7 +14917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:38" hidden="1">
       <c r="A64" s="4" t="s">
         <v>1</v>
       </c>
@@ -14983,7 +14990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:38">
+    <row r="65" spans="1:38" hidden="1">
       <c r="A65" s="4" t="s">
         <v>1</v>
       </c>
@@ -15054,7 +15061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:38" hidden="1">
       <c r="A66" s="4" t="s">
         <v>249</v>
       </c>
@@ -15152,7 +15159,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="67" spans="1:38">
+    <row r="67" spans="1:38" hidden="1">
       <c r="A67" s="4" t="s">
         <v>8</v>
       </c>
@@ -15239,7 +15246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:38">
+    <row r="68" spans="1:38" hidden="1">
       <c r="A68" s="4" t="s">
         <v>8</v>
       </c>
@@ -15312,7 +15319,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:38" hidden="1">
       <c r="A69" s="4" t="s">
         <v>8</v>
       </c>
@@ -15385,7 +15392,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:38" hidden="1">
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
@@ -15456,7 +15463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:38" hidden="1">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -15527,7 +15534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:38">
+    <row r="72" spans="1:38" hidden="1">
       <c r="A72" s="4" t="s">
         <v>10</v>
       </c>
@@ -15600,7 +15607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:38" hidden="1">
       <c r="A73" s="4" t="s">
         <v>14</v>
       </c>
@@ -15677,7 +15684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:38" hidden="1">
       <c r="A74" s="4" t="s">
         <v>14</v>
       </c>
@@ -15750,7 +15757,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:38" hidden="1">
       <c r="A75" s="4" t="s">
         <v>14</v>
       </c>
@@ -15823,7 +15830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:38" hidden="1">
       <c r="A76" s="4" t="s">
         <v>15</v>
       </c>
@@ -15910,7 +15917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:38">
+    <row r="77" spans="1:38" hidden="1">
       <c r="A77" s="4" t="s">
         <v>15</v>
       </c>
@@ -15983,7 +15990,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:38">
+    <row r="78" spans="1:38" hidden="1">
       <c r="A78" s="4" t="s">
         <v>15</v>
       </c>
@@ -16056,7 +16063,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:38">
+    <row r="79" spans="1:38" hidden="1">
       <c r="A79" s="4" t="s">
         <v>15</v>
       </c>
@@ -16127,7 +16134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:38">
+    <row r="80" spans="1:38" hidden="1">
       <c r="A80" s="4" t="s">
         <v>15</v>
       </c>
@@ -16198,7 +16205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:38">
+    <row r="81" spans="1:38" hidden="1">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
@@ -16279,7 +16286,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="82" spans="1:38">
+    <row r="82" spans="1:38" hidden="1">
       <c r="A82" s="4" t="s">
         <v>16</v>
       </c>
@@ -16350,7 +16357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:38">
+    <row r="83" spans="1:38" hidden="1">
       <c r="A83" s="4" t="s">
         <v>18</v>
       </c>
@@ -16441,7 +16448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:38">
+    <row r="84" spans="1:38" hidden="1">
       <c r="A84" s="4" t="s">
         <v>24</v>
       </c>
@@ -16514,7 +16521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:38">
+    <row r="85" spans="1:38" hidden="1">
       <c r="A85" s="4" t="s">
         <v>24</v>
       </c>
@@ -16587,7 +16594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:38">
+    <row r="86" spans="1:38" hidden="1">
       <c r="A86" s="4" t="s">
         <v>24</v>
       </c>
@@ -16660,7 +16667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:38">
+    <row r="87" spans="1:38" hidden="1">
       <c r="A87" s="4" t="s">
         <v>24</v>
       </c>
@@ -16733,7 +16740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:38">
+    <row r="88" spans="1:38" hidden="1">
       <c r="A88" s="8" t="s">
         <v>21</v>
       </c>
@@ -16804,7 +16811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:38">
+    <row r="89" spans="1:38" hidden="1">
       <c r="A89" s="8" t="s">
         <v>21</v>
       </c>
@@ -16875,7 +16882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:38">
+    <row r="90" spans="1:38" hidden="1">
       <c r="A90" s="3" t="s">
         <v>109</v>
       </c>
@@ -16966,7 +16973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:38">
+    <row r="91" spans="1:38" hidden="1">
       <c r="A91" s="3" t="s">
         <v>109</v>
       </c>
@@ -17037,7 +17044,7 @@
         <v>5.6000000000000005</v>
       </c>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:38" hidden="1">
       <c r="A92" s="3" t="s">
         <v>109</v>
       </c>
@@ -17112,7 +17119,7 @@
         <v>18.400000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:38" hidden="1">
       <c r="A93" s="3" t="s">
         <v>191</v>
       </c>
@@ -17183,7 +17190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:38">
+    <row r="94" spans="1:38" hidden="1">
       <c r="A94" s="3" t="s">
         <v>111</v>
       </c>
@@ -17254,7 +17261,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="95" spans="1:38">
+    <row r="95" spans="1:38" hidden="1">
       <c r="A95" s="3" t="s">
         <v>111</v>
       </c>
@@ -17325,7 +17332,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="96" spans="1:38">
+    <row r="96" spans="1:38" hidden="1">
       <c r="A96" s="3" t="s">
         <v>192</v>
       </c>
@@ -17398,7 +17405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:38">
+    <row r="97" spans="1:38" hidden="1">
       <c r="A97" s="3" t="s">
         <v>192</v>
       </c>
@@ -17471,7 +17478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:38">
+    <row r="98" spans="1:38" hidden="1">
       <c r="A98" s="3" t="s">
         <v>112</v>
       </c>
@@ -17544,7 +17551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:38">
+    <row r="99" spans="1:38" hidden="1">
       <c r="A99" s="3" t="s">
         <v>112</v>
       </c>
@@ -17617,7 +17624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:38">
+    <row r="100" spans="1:38" hidden="1">
       <c r="A100" s="3" t="s">
         <v>112</v>
       </c>
@@ -17690,7 +17697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:38">
+    <row r="101" spans="1:38" hidden="1">
       <c r="A101" s="3" t="s">
         <v>103</v>
       </c>
@@ -17761,7 +17768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:38">
+    <row r="102" spans="1:38" hidden="1">
       <c r="A102" s="3" t="s">
         <v>105</v>
       </c>
@@ -17832,7 +17839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:38">
+    <row r="103" spans="1:38" hidden="1">
       <c r="A103" s="3" t="s">
         <v>107</v>
       </c>
@@ -17913,7 +17920,7 @@
         <v>23</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D104" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -18025,7 +18032,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="1:38">
+    <row r="105" spans="1:38" hidden="1">
       <c r="A105" s="9" t="s">
         <v>48</v>
       </c>
@@ -18102,7 +18109,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="106" spans="1:38">
+    <row r="106" spans="1:38" hidden="1">
       <c r="A106" s="9" t="s">
         <v>48</v>
       </c>
@@ -18325,7 +18332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:38">
+    <row r="109" spans="1:38" hidden="1">
       <c r="A109" s="9" t="s">
         <v>48</v>
       </c>
@@ -18398,7 +18405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:38">
+    <row r="110" spans="1:38" hidden="1">
       <c r="A110" s="4" t="s">
         <v>64</v>
       </c>
@@ -18499,7 +18506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:38">
+    <row r="111" spans="1:38" hidden="1">
       <c r="A111" s="4" t="s">
         <v>64</v>
       </c>
@@ -18570,7 +18577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:38">
+    <row r="112" spans="1:38" hidden="1">
       <c r="A112" s="4" t="s">
         <v>239</v>
       </c>
@@ -18641,7 +18648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:38">
+    <row r="113" spans="1:38" hidden="1">
       <c r="A113" s="4" t="s">
         <v>239</v>
       </c>
@@ -18712,7 +18719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:38">
+    <row r="114" spans="1:38" hidden="1">
       <c r="A114" s="4" t="s">
         <v>66</v>
       </c>
@@ -18785,7 +18792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:38">
+    <row r="115" spans="1:38" hidden="1">
       <c r="A115" s="4" t="s">
         <v>66</v>
       </c>
@@ -18856,7 +18863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:38">
+    <row r="116" spans="1:38" hidden="1">
       <c r="A116" s="4" t="s">
         <v>69</v>
       </c>
@@ -18943,7 +18950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:38">
+    <row r="117" spans="1:38" hidden="1">
       <c r="A117" s="4" t="s">
         <v>69</v>
       </c>
@@ -19016,7 +19023,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="118" spans="1:38">
+    <row r="118" spans="1:38" hidden="1">
       <c r="A118" s="4" t="s">
         <v>72</v>
       </c>
@@ -19103,7 +19110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:38">
+    <row r="119" spans="1:38" hidden="1">
       <c r="A119" s="4" t="s">
         <v>72</v>
       </c>
@@ -19247,7 +19254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:38">
+    <row r="121" spans="1:38" hidden="1">
       <c r="A121" s="4" t="s">
         <v>74</v>
       </c>
@@ -19338,7 +19345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:38">
+    <row r="122" spans="1:38" hidden="1">
       <c r="A122" s="4" t="s">
         <v>74</v>
       </c>
@@ -19415,7 +19422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:38">
+    <row r="123" spans="1:38" hidden="1">
       <c r="A123" s="3" t="s">
         <v>193</v>
       </c>
@@ -19486,7 +19493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:38">
+    <row r="124" spans="1:38" hidden="1">
       <c r="A124" s="3" t="s">
         <v>194</v>
       </c>
@@ -19559,7 +19566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:38">
+    <row r="125" spans="1:38" hidden="1">
       <c r="A125" s="3" t="s">
         <v>195</v>
       </c>
@@ -19650,7 +19657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:38">
+    <row r="126" spans="1:38" hidden="1">
       <c r="A126" s="3" t="s">
         <v>195</v>
       </c>
@@ -19721,7 +19728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:38">
+    <row r="127" spans="1:38" hidden="1">
       <c r="A127" s="3" t="s">
         <v>195</v>
       </c>
@@ -19794,7 +19801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:38">
+    <row r="128" spans="1:38" hidden="1">
       <c r="A128" s="3" t="s">
         <v>196</v>
       </c>
@@ -19875,7 +19882,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="129" spans="1:38">
+    <row r="129" spans="1:38" hidden="1">
       <c r="A129" s="3" t="s">
         <v>196</v>
       </c>
@@ -19956,7 +19963,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="130" spans="1:38">
+    <row r="130" spans="1:38" hidden="1">
       <c r="A130" s="3" t="s">
         <v>117</v>
       </c>
@@ -20027,7 +20034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:38">
+    <row r="131" spans="1:38" hidden="1">
       <c r="A131" s="3" t="s">
         <v>117</v>
       </c>
@@ -20098,7 +20105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:38">
+    <row r="132" spans="1:38" hidden="1">
       <c r="A132" s="3" t="s">
         <v>117</v>
       </c>
@@ -20169,7 +20176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:38">
+    <row r="133" spans="1:38" hidden="1">
       <c r="A133" s="3" t="s">
         <v>240</v>
       </c>
@@ -20260,7 +20267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:38">
+    <row r="134" spans="1:38" hidden="1">
       <c r="A134" s="3" t="s">
         <v>240</v>
       </c>
@@ -20333,7 +20340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:38">
+    <row r="135" spans="1:38" hidden="1">
       <c r="A135" s="3" t="s">
         <v>119</v>
       </c>
@@ -20424,7 +20431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:38">
+    <row r="136" spans="1:38" hidden="1">
       <c r="A136" s="3" t="s">
         <v>71</v>
       </c>
@@ -20497,7 +20504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:38">
+    <row r="137" spans="1:38" hidden="1">
       <c r="A137" s="3" t="s">
         <v>197</v>
       </c>
@@ -20570,7 +20577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:38">
+    <row r="138" spans="1:38" hidden="1">
       <c r="A138" s="3" t="s">
         <v>197</v>
       </c>
@@ -20641,7 +20648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:38">
+    <row r="139" spans="1:38" hidden="1">
       <c r="A139" s="3" t="s">
         <v>198</v>
       </c>
@@ -20712,7 +20719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:38">
+    <row r="140" spans="1:38" hidden="1">
       <c r="A140" s="3" t="s">
         <v>198</v>
       </c>
@@ -20783,7 +20790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:38">
+    <row r="141" spans="1:38" hidden="1">
       <c r="A141" s="3" t="s">
         <v>198</v>
       </c>
@@ -20862,7 +20869,7 @@
         <v>23</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D142" s="29">
         <f>INDEX(Table2[CA weight],MATCH(Table1[[#This Row],[Module Code]],Table2[Module Code],0))</f>
@@ -20974,7 +20981,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="143" spans="1:38">
+    <row r="143" spans="1:38" hidden="1">
       <c r="A143" s="4" t="s">
         <v>77</v>
       </c>
@@ -21051,7 +21058,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="144" spans="1:38">
+    <row r="144" spans="1:38" hidden="1">
       <c r="A144" s="4" t="s">
         <v>77</v>
       </c>
@@ -21347,7 +21354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:38">
+    <row r="148" spans="1:38" hidden="1">
       <c r="A148" s="4" t="s">
         <v>77</v>
       </c>
@@ -21420,7 +21427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:38">
+    <row r="149" spans="1:38" hidden="1">
       <c r="A149" s="4" t="s">
         <v>77</v>
       </c>
@@ -21493,7 +21500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:38">
+    <row r="150" spans="1:38" hidden="1">
       <c r="A150" s="4" t="s">
         <v>245</v>
       </c>
@@ -21564,7 +21571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:38">
+    <row r="151" spans="1:38" hidden="1">
       <c r="A151" s="4" t="s">
         <v>245</v>
       </c>
@@ -21635,7 +21642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:38">
+    <row r="152" spans="1:38" hidden="1">
       <c r="A152" s="4" t="s">
         <v>245</v>
       </c>
@@ -21706,7 +21713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:38">
+    <row r="153" spans="1:38" hidden="1">
       <c r="A153" s="4" t="s">
         <v>247</v>
       </c>
@@ -21779,7 +21786,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="154" spans="1:38">
+    <row r="154" spans="1:38" hidden="1">
       <c r="A154" s="4" t="s">
         <v>243</v>
       </c>
@@ -21868,7 +21875,7 @@
         <v>19.999999999999996</v>
       </c>
     </row>
-    <row r="155" spans="1:38">
+    <row r="155" spans="1:38" hidden="1">
       <c r="A155" s="4" t="s">
         <v>243</v>
       </c>
@@ -21957,7 +21964,7 @@
         <v>7.9999999999999982</v>
       </c>
     </row>
-    <row r="156" spans="1:38">
+    <row r="156" spans="1:38" hidden="1">
       <c r="A156" s="4" t="s">
         <v>243</v>
       </c>
@@ -22028,7 +22035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:38">
+    <row r="157" spans="1:38" hidden="1">
       <c r="A157" s="4" t="s">
         <v>184</v>
       </c>
@@ -22099,7 +22106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:38">
+    <row r="158" spans="1:38" hidden="1">
       <c r="A158" s="4" t="s">
         <v>184</v>
       </c>
@@ -22170,7 +22177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:38">
+    <row r="159" spans="1:38" hidden="1">
       <c r="A159" s="4" t="s">
         <v>184</v>
       </c>
@@ -22314,7 +22321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:38">
+    <row r="161" spans="1:38" hidden="1">
       <c r="A161" s="4" t="s">
         <v>184</v>
       </c>
@@ -22387,7 +22394,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="162" spans="1:38">
+    <row r="162" spans="1:38" hidden="1">
       <c r="A162" s="4" t="s">
         <v>184</v>
       </c>
@@ -22460,7 +22467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:38">
+    <row r="163" spans="1:38" hidden="1">
       <c r="A163" s="4" t="s">
         <v>185</v>
       </c>
@@ -22604,7 +22611,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="165" spans="1:38">
+    <row r="165" spans="1:38" hidden="1">
       <c r="A165" s="4" t="s">
         <v>185</v>
       </c>
@@ -22746,7 +22753,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:38">
+    <row r="167" spans="1:38" hidden="1">
       <c r="A167" s="3" t="s">
         <v>275</v>
       </c>
@@ -22817,7 +22824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:38">
+    <row r="168" spans="1:38" hidden="1">
       <c r="A168" s="3" t="s">
         <v>275</v>
       </c>
@@ -22888,7 +22895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:38">
+    <row r="169" spans="1:38" hidden="1">
       <c r="A169" s="3" t="s">
         <v>279</v>
       </c>
@@ -22959,7 +22966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:38">
+    <row r="170" spans="1:38" hidden="1">
       <c r="A170" s="3" t="s">
         <v>279</v>
       </c>
@@ -23030,7 +23037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:38">
+    <row r="171" spans="1:38" hidden="1">
       <c r="A171" s="3" t="s">
         <v>279</v>
       </c>
@@ -23101,7 +23108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:38">
+    <row r="172" spans="1:38" hidden="1">
       <c r="A172" s="3" t="s">
         <v>281</v>
       </c>
@@ -23174,7 +23181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:38">
+    <row r="173" spans="1:38" hidden="1">
       <c r="A173" s="3" t="s">
         <v>281</v>
       </c>
@@ -23247,7 +23254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:38">
+    <row r="174" spans="1:38" hidden="1">
       <c r="A174" s="3" t="s">
         <v>282</v>
       </c>

</xml_diff>

<commit_message>
tweak plot legend for portfolios
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1597" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88961667-058C-436B-B343-B9958A234E38}"/>
+  <xr:revisionPtr revIDLastSave="1601" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401D57D5-BC21-4268-9572-FD6793AE0922}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="26115" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1136,18 +1136,12 @@
     <t>Weekly task</t>
   </si>
   <si>
-    <t>Weekly Tests</t>
-  </si>
-  <si>
     <t>Tests Portfolio</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Weekly tests</t>
-  </si>
-  <si>
     <t>Tests Portfolio 1</t>
   </si>
   <si>
@@ -1163,9 +1157,6 @@
     <t>Quiz Deadline</t>
   </si>
   <si>
-    <t>Weekly Quizzez</t>
-  </si>
-  <si>
     <t>Final Report</t>
   </si>
   <si>
@@ -1182,6 +1173,15 @@
   </si>
   <si>
     <t>CA1 (*)</t>
+  </si>
+  <si>
+    <t>Weekly Tests (P)</t>
+  </si>
+  <si>
+    <t>Weekly tests (P)</t>
+  </si>
+  <si>
+    <t>Weekly Quizzes (P)</t>
   </si>
 </sst>
 </file>
@@ -9069,7 +9069,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9987,10 +9987,10 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C103" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K123" sqref="K123"/>
+      <selection pane="bottomRight" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10367,7 +10367,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>222</v>
@@ -10440,7 +10440,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>231</v>
@@ -10746,7 +10746,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>222</v>
@@ -13264,7 +13264,7 @@
         <v>20</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>222</v>
@@ -13752,7 +13752,7 @@
         <v>20</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>222</v>
@@ -14086,7 +14086,7 @@
         <v>20</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>231</v>
@@ -15235,13 +15235,13 @@
         <v>20</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="G67" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I67" s="11">
         <v>1</v>
@@ -15326,7 +15326,7 @@
         <v>20</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>231</v>
@@ -15568,13 +15568,13 @@
         <v>10</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I71" s="11">
         <v>1</v>
@@ -15655,7 +15655,7 @@
         <v>10</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>231</v>
@@ -15728,7 +15728,7 @@
         <v>10</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G73" s="11" t="s">
         <v>231</v>
@@ -16239,13 +16239,13 @@
         <v>10</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I80" s="11">
         <v>1</v>
@@ -16326,7 +16326,7 @@
         <v>10</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>231</v>
@@ -16399,7 +16399,7 @@
         <v>10</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>231</v>
@@ -17283,13 +17283,13 @@
         <v>20</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I94" s="11">
         <v>1</v>
@@ -17374,7 +17374,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>231</v>
@@ -19349,7 +19349,7 @@
         <v>10</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>222</v>
@@ -19436,7 +19436,7 @@
         <v>10</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>231</v>
@@ -19507,7 +19507,7 @@
         <v>10</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
add best of notes
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1607" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BB3883-1612-4C30-AB0C-C4914339E050}"/>
+  <xr:revisionPtr revIDLastSave="1628" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5E8C72-59EA-4D03-9092-9C67FC1377AB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="12877" yWindow="0" windowWidth="13125" windowHeight="15563" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId5"/>
+    <pivotCache cacheId="17" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="385">
   <si>
     <t>Module Code</t>
   </si>
@@ -1034,9 +1034,6 @@
     <t>Final Report (U/D)</t>
   </si>
   <si>
-    <t>Quiz (*)</t>
-  </si>
-  <si>
     <t>Tu/Fr</t>
   </si>
   <si>
@@ -1061,9 +1058,6 @@
     <t>ML Methods</t>
   </si>
   <si>
-    <t>Wiley Test</t>
-  </si>
-  <si>
     <t>Portfolio (P)</t>
   </si>
   <si>
@@ -1082,12 +1076,6 @@
     <t>Group Project</t>
   </si>
   <si>
-    <t>Weekly Tests 1</t>
-  </si>
-  <si>
-    <t>Weekly Tests 2</t>
-  </si>
-  <si>
     <t>Mini Project</t>
   </si>
   <si>
@@ -1133,9 +1121,6 @@
     <t>Performance (P)</t>
   </si>
   <si>
-    <t>Weekly task</t>
-  </si>
-  <si>
     <t>Tests Portfolio</t>
   </si>
   <si>
@@ -1163,12 +1148,6 @@
     <t>Weekly Quiz (P)</t>
   </si>
   <si>
-    <t>Lab Attendance</t>
-  </si>
-  <si>
-    <t>Wiley Quiz</t>
-  </si>
-  <si>
     <t>Formative Quiz</t>
   </si>
   <si>
@@ -1181,10 +1160,43 @@
     <t>Weekly tests (P)</t>
   </si>
   <si>
-    <t>Weekly Quizzes (P)</t>
-  </si>
-  <si>
     <t>Python exercise (*)</t>
+  </si>
+  <si>
+    <t>Wiley Quiz (6 of 9)</t>
+  </si>
+  <si>
+    <t>Wiley Test (best 8)</t>
+  </si>
+  <si>
+    <t>Quiz (best 6)</t>
+  </si>
+  <si>
+    <t>Weekly task (best 6)</t>
+  </si>
+  <si>
+    <t>Quiz (best 3)</t>
+  </si>
+  <si>
+    <t>Quiz (best 5)</t>
+  </si>
+  <si>
+    <t>Weekly Quiz (best 7)</t>
+  </si>
+  <si>
+    <t>Quiz (*) (best 5)</t>
+  </si>
+  <si>
+    <t>Weekly Test 1 (best 3)</t>
+  </si>
+  <si>
+    <t>Weekly Test 2 (best 3)</t>
+  </si>
+  <si>
+    <t>Quiz (best 65)</t>
+  </si>
+  <si>
+    <t>Lab Engagement</t>
   </si>
 </sst>
 </file>
@@ -9072,7 +9084,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9990,27 +10002,27 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.7265625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.7265625" style="10" customWidth="1"/>
-    <col min="12" max="23" width="9.08984375" style="14" customWidth="1"/>
-    <col min="24" max="36" width="9.08984375" style="16"/>
+    <col min="6" max="6" width="21.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" style="10" customWidth="1"/>
+    <col min="12" max="23" width="9.140625" style="14" customWidth="1"/>
+    <col min="24" max="36" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="44" customFormat="1" ht="29">
+    <row r="1" spans="1:38" s="44" customFormat="1" ht="30">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -10370,7 +10382,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>222</v>
@@ -10443,7 +10455,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>231</v>
@@ -10749,7 +10761,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>222</v>
@@ -10943,7 +10955,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>231</v>
@@ -11089,7 +11101,7 @@
         <v>20</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>339</v>
+        <v>374</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>231</v>
@@ -11186,7 +11198,7 @@
         <v>231</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I15" s="11">
         <v>1</v>
@@ -11863,7 +11875,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>255</v>
+        <v>375</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>231</v>
@@ -12890,7 +12902,7 @@
         <v>10</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>231</v>
@@ -13042,7 +13054,7 @@
         <v>10</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>231</v>
@@ -13267,7 +13279,7 @@
         <v>20</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>222</v>
@@ -13755,7 +13767,7 @@
         <v>20</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>222</v>
@@ -14089,7 +14101,7 @@
         <v>20</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>231</v>
@@ -14160,7 +14172,7 @@
         <v>20</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>255</v>
+        <v>375</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>231</v>
@@ -14401,7 +14413,7 @@
         <v>10</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>255</v>
+        <v>375</v>
       </c>
       <c r="G56" s="11" t="s">
         <v>231</v>
@@ -14865,7 +14877,7 @@
         <v>10</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>231</v>
@@ -15238,13 +15250,13 @@
         <v>20</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G67" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I67" s="11">
         <v>1</v>
@@ -15329,7 +15341,7 @@
         <v>20</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>231</v>
@@ -15473,7 +15485,7 @@
         <v>10</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>231</v>
@@ -15571,13 +15583,13 @@
         <v>10</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I71" s="11">
         <v>1</v>
@@ -15658,7 +15670,7 @@
         <v>10</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>231</v>
@@ -15731,7 +15743,7 @@
         <v>10</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="G73" s="11" t="s">
         <v>231</v>
@@ -16242,13 +16254,13 @@
         <v>10</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I80" s="11">
         <v>1</v>
@@ -16329,7 +16341,7 @@
         <v>10</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>231</v>
@@ -16402,7 +16414,7 @@
         <v>10</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>231</v>
@@ -16617,7 +16629,7 @@
         <v>10</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>255</v>
+        <v>377</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>231</v>
@@ -16769,7 +16781,7 @@
         <v>10</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>255</v>
+        <v>378</v>
       </c>
       <c r="G87" s="11" t="s">
         <v>231</v>
@@ -17073,7 +17085,7 @@
         <v>10</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>231</v>
@@ -17125,7 +17137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:38" ht="28.5">
       <c r="A92" s="8" t="s">
         <v>21</v>
       </c>
@@ -17196,7 +17208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:38" ht="28.5">
       <c r="A93" s="8" t="s">
         <v>21</v>
       </c>
@@ -17292,7 +17304,7 @@
         <v>222</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I94" s="11">
         <v>1</v>
@@ -17377,7 +17389,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>231</v>
@@ -17807,7 +17819,7 @@
         <v>10</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>231</v>
@@ -17878,7 +17890,7 @@
         <v>10</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>231</v>
@@ -18805,7 +18817,7 @@
         <v>10</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>255</v>
+        <v>375</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>231</v>
@@ -19192,7 +19204,7 @@
         <v>10</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>231</v>
@@ -19352,7 +19364,7 @@
         <v>10</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>222</v>
@@ -19439,7 +19451,7 @@
         <v>10</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>231</v>
@@ -19510,7 +19522,7 @@
         <v>10</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>231</v>
@@ -19654,7 +19666,7 @@
         <v>10</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>330</v>
+        <v>380</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>231</v>
@@ -19966,7 +19978,7 @@
         <v>10</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>255</v>
+        <v>378</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>231</v>
@@ -20201,7 +20213,7 @@
         <v>10</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>346</v>
+        <v>381</v>
       </c>
       <c r="G132" s="11" t="s">
         <v>231</v>
@@ -20282,7 +20294,7 @@
         <v>10</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="G133" s="11" t="s">
         <v>231</v>
@@ -20576,7 +20588,7 @@
         <v>10</v>
       </c>
       <c r="F137" s="12" t="s">
-        <v>255</v>
+        <v>378</v>
       </c>
       <c r="G137" s="11" t="s">
         <v>231</v>
@@ -20740,7 +20752,7 @@
         <v>10</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>255</v>
+        <v>383</v>
       </c>
       <c r="G139" s="11" t="s">
         <v>231</v>
@@ -20831,7 +20843,7 @@
         <v>10</v>
       </c>
       <c r="F140" s="12" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G140" s="11" t="s">
         <v>231</v>
@@ -21119,7 +21131,7 @@
         <v>10</v>
       </c>
       <c r="F144" s="12" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G144" s="11" t="s">
         <v>231</v>
@@ -21190,7 +21202,7 @@
         <v>10</v>
       </c>
       <c r="F145" s="12" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G145" s="11" t="s">
         <v>231</v>
@@ -21458,7 +21470,7 @@
         <v>60</v>
       </c>
       <c r="F148" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G148" s="11" t="s">
         <v>231</v>
@@ -21531,7 +21543,7 @@
         <v>60</v>
       </c>
       <c r="F149" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G149" s="11" t="s">
         <v>231</v>
@@ -21677,7 +21689,7 @@
         <v>60</v>
       </c>
       <c r="F151" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G151" s="11" t="s">
         <v>231</v>
@@ -21823,7 +21835,7 @@
         <v>60</v>
       </c>
       <c r="F153" s="37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G153" s="11" t="s">
         <v>231</v>
@@ -22182,7 +22194,7 @@
         <v>10</v>
       </c>
       <c r="F158" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G158" s="11" t="s">
         <v>231</v>
@@ -22271,7 +22283,7 @@
         <v>10</v>
       </c>
       <c r="F159" s="11" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G159" s="11" t="s">
         <v>231</v>
@@ -22360,7 +22372,7 @@
         <v>10</v>
       </c>
       <c r="F160" s="11" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G160" s="11" t="s">
         <v>231</v>
@@ -22431,7 +22443,7 @@
         <v>20</v>
       </c>
       <c r="F161" s="11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G161" s="11" t="s">
         <v>231</v>
@@ -22502,7 +22514,7 @@
         <v>20</v>
       </c>
       <c r="F162" s="11" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G162" s="11" t="s">
         <v>231</v>
@@ -22573,7 +22585,7 @@
         <v>20</v>
       </c>
       <c r="F163" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G163" s="11" t="s">
         <v>231</v>
@@ -22644,7 +22656,7 @@
         <v>20</v>
       </c>
       <c r="F164" s="11" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G164" s="11" t="s">
         <v>231</v>
@@ -22717,7 +22729,7 @@
         <v>20</v>
       </c>
       <c r="F165" s="11" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G165" s="11" t="s">
         <v>231</v>
@@ -22790,7 +22802,7 @@
         <v>20</v>
       </c>
       <c r="F166" s="11" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G166" s="11" t="s">
         <v>231</v>
@@ -22863,7 +22875,7 @@
         <v>20</v>
       </c>
       <c r="F167" s="11" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G167" s="11" t="s">
         <v>231</v>
@@ -22934,7 +22946,7 @@
         <v>20</v>
       </c>
       <c r="F168" s="11" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G168" s="11" t="s">
         <v>231</v>
@@ -23007,7 +23019,7 @@
         <v>20</v>
       </c>
       <c r="F169" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G169" s="11" t="s">
         <v>231</v>
@@ -23078,7 +23090,7 @@
         <v>20</v>
       </c>
       <c r="F170" s="11" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G170" s="11" t="s">
         <v>231</v>
@@ -23155,7 +23167,7 @@
         <v>231</v>
       </c>
       <c r="H171" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I171" s="11">
         <v>4</v>
@@ -23226,7 +23238,7 @@
         <v>231</v>
       </c>
       <c r="H172" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I172" s="11">
         <v>6</v>
@@ -23504,7 +23516,7 @@
         <v>20</v>
       </c>
       <c r="F176" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G176" s="11" t="s">
         <v>231</v>
@@ -23577,7 +23589,7 @@
         <v>20</v>
       </c>
       <c r="F177" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G177" s="11" t="s">
         <v>231</v>
@@ -23650,7 +23662,7 @@
         <v>20</v>
       </c>
       <c r="F178" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G178" s="11" t="s">
         <v>231</v>
@@ -23725,16 +23737,16 @@
       <selection pane="bottomRight" activeCell="X64" sqref="X64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="10" customWidth="1"/>
-    <col min="7" max="15" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="8.7265625" style="16"/>
+    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
+    <col min="7" max="15" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="17.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="8.7109375" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -27056,7 +27068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" ht="28.5">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -29884,14 +29896,14 @@
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="5" customWidth="1"/>
   </cols>
@@ -31705,7 +31717,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" ht="28.5">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -35314,11 +35326,11 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
tweaked best of notes
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1628" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5E8C72-59EA-4D03-9092-9C67FC1377AB}"/>
+  <xr:revisionPtr revIDLastSave="1643" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F52F4F-F15D-473F-BA92-783EA6922A6B}"/>
   <bookViews>
     <workbookView xWindow="12877" yWindow="0" windowWidth="13125" windowHeight="15563" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="386">
   <si>
     <t>Module Code</t>
   </si>
@@ -1166,37 +1166,40 @@
     <t>Wiley Quiz (6 of 9)</t>
   </si>
   <si>
-    <t>Wiley Test (best 8)</t>
-  </si>
-  <si>
     <t>Quiz (best 6)</t>
   </si>
   <si>
-    <t>Weekly task (best 6)</t>
-  </si>
-  <si>
-    <t>Quiz (best 3)</t>
-  </si>
-  <si>
-    <t>Quiz (best 5)</t>
-  </si>
-  <si>
-    <t>Weekly Quiz (best 7)</t>
-  </si>
-  <si>
-    <t>Quiz (*) (best 5)</t>
-  </si>
-  <si>
-    <t>Weekly Test 1 (best 3)</t>
-  </si>
-  <si>
-    <t>Weekly Test 2 (best 3)</t>
-  </si>
-  <si>
-    <t>Quiz (best 65)</t>
-  </si>
-  <si>
     <t>Lab Engagement</t>
+  </si>
+  <si>
+    <t>Wiley Test (8 of 10)</t>
+  </si>
+  <si>
+    <t>Quiz (6 of 10)</t>
+  </si>
+  <si>
+    <t>Weekly task (6 of 9)</t>
+  </si>
+  <si>
+    <t>Quiz (3 of 5)</t>
+  </si>
+  <si>
+    <t>Quiz (5 of 10)</t>
+  </si>
+  <si>
+    <t>Weekly Quiz (7 of 10)</t>
+  </si>
+  <si>
+    <t>Weekly task (6 of 8)</t>
+  </si>
+  <si>
+    <t>Quiz (*) (5 of 10)</t>
+  </si>
+  <si>
+    <t>Weekly Test 1 (3 of 5)</t>
+  </si>
+  <si>
+    <t>Weekly Test 2 (3 of 5)</t>
   </si>
 </sst>
 </file>
@@ -10002,10 +10005,10 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F49" sqref="F49"/>
+      <selection pane="bottomRight" activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10761,7 +10764,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>222</v>
@@ -11101,7 +11104,7 @@
         <v>20</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>231</v>
@@ -11875,7 +11878,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>231</v>
@@ -13279,7 +13282,7 @@
         <v>20</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>222</v>
@@ -13767,7 +13770,7 @@
         <v>20</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>222</v>
@@ -14172,7 +14175,7 @@
         <v>20</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>231</v>
@@ -14413,7 +14416,7 @@
         <v>10</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G56" s="11" t="s">
         <v>231</v>
@@ -15485,7 +15488,7 @@
         <v>10</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>231</v>
@@ -16629,7 +16632,7 @@
         <v>10</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>231</v>
@@ -16781,7 +16784,7 @@
         <v>10</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G87" s="11" t="s">
         <v>231</v>
@@ -17298,7 +17301,7 @@
         <v>20</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>222</v>
@@ -18817,7 +18820,7 @@
         <v>10</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>231</v>
@@ -19204,7 +19207,7 @@
         <v>10</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>231</v>
@@ -19666,7 +19669,7 @@
         <v>10</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>231</v>
@@ -19978,7 +19981,7 @@
         <v>10</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>231</v>
@@ -20213,7 +20216,7 @@
         <v>10</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="G132" s="11" t="s">
         <v>231</v>
@@ -20294,7 +20297,7 @@
         <v>10</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="G133" s="11" t="s">
         <v>231</v>
@@ -20588,7 +20591,7 @@
         <v>10</v>
       </c>
       <c r="F137" s="12" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G137" s="11" t="s">
         <v>231</v>
@@ -20752,7 +20755,7 @@
         <v>10</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G139" s="11" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
tweaked PX4310 workload week 1
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1643" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F52F4F-F15D-473F-BA92-783EA6922A6B}"/>
+  <xr:revisionPtr revIDLastSave="1644" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C08CAA0-3ABD-4891-9927-8D5D256A39D0}"/>
   <bookViews>
-    <workbookView xWindow="12877" yWindow="0" windowWidth="13125" windowHeight="15563" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" activeTab="1" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -10004,8 +10004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66039B40-29AD-4D93-B125-EAF72A7B3996}">
   <dimension ref="A1:AL178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F114" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F140" sqref="F140"/>
@@ -23733,11 +23733,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0482654D-1732-43E5-85EC-021407B07CE5}">
   <dimension ref="A1:AE141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X64" sqref="X64"/>
+      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29472,7 +29472,7 @@
         <v>0.5</v>
       </c>
       <c r="G61" s="31">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="H61" s="31">
         <v>1</v>
@@ -29543,7 +29543,7 @@
       </c>
       <c r="AE61" s="37">
         <f>SUM(Table14[[#This Row],[Autumn Week 1]:[Spring Week 12]])</f>
-        <v>29.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="62" spans="1:31">
@@ -36881,15 +36881,15 @@
       </c>
       <c r="D67">
         <f>INDEX(Table14[Total],MATCH(Sheet2!A67,Table14[Module Code],0))</f>
-        <v>29.5</v>
+        <v>12.5</v>
       </c>
       <c r="E67">
         <f t="shared" si="0"/>
-        <v>530.90000000000009</v>
+        <v>513.90000000000009</v>
       </c>
       <c r="F67">
         <f t="shared" si="1"/>
-        <v>8.8483333333333345</v>
+        <v>8.5650000000000013</v>
       </c>
     </row>
     <row r="68" spans="1:6">

</xml_diff>

<commit_message>
updated PX3155 day and removed 'U/D' notes
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1647" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB13DD57-D680-47C8-935D-EB6FCBBDD55A}"/>
+  <xr:revisionPtr revIDLastSave="1656" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C133DB0C-B249-4B27-8DCF-17BA242244FC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" activeTab="2" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="269" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="382">
   <si>
     <t>Module Code</t>
   </si>
@@ -977,33 +977,21 @@
     <t>(TBC)</t>
   </si>
   <si>
-    <t>AstroPhoto (U/D)</t>
-  </si>
-  <si>
     <t>CA2 (U/D)</t>
   </si>
   <si>
     <t>Mo/Th</t>
   </si>
   <si>
-    <t>Assignment (U/D)</t>
-  </si>
-  <si>
     <t>CA (U/D)</t>
   </si>
   <si>
-    <t>Presentation (U/D)</t>
-  </si>
-  <si>
     <t>Poster Pres (*)</t>
   </si>
   <si>
     <t>Th/Fr</t>
   </si>
   <si>
-    <t>Lab Diary (*) (U/D)</t>
-  </si>
-  <si>
     <t>Workshops (*)</t>
   </si>
   <si>
@@ -1028,21 +1016,9 @@
     <t>Pres (*) (+/- 1wk)</t>
   </si>
   <si>
-    <t>Final Diary (U/D)</t>
-  </si>
-  <si>
-    <t>Final Report (U/D)</t>
-  </si>
-  <si>
     <t>Tu/Fr</t>
   </si>
   <si>
-    <t>Project Diary (U/D)</t>
-  </si>
-  <si>
-    <t>Project Report (U/D)</t>
-  </si>
-  <si>
     <t>Viva (*)</t>
   </si>
   <si>
@@ -1200,6 +1176,18 @@
   </si>
   <si>
     <t>Weekly Test 2 (3 of 5)</t>
+  </si>
+  <si>
+    <t>Project Report</t>
+  </si>
+  <si>
+    <t>Project Diary</t>
+  </si>
+  <si>
+    <t>Final Diary</t>
+  </si>
+  <si>
+    <t>AstroPhoto</t>
   </si>
 </sst>
 </file>
@@ -9087,7 +9075,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="269" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -10004,28 +9992,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66039B40-29AD-4D93-B125-EAF72A7B3996}">
   <dimension ref="A1:AL178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C152" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I143" sqref="I143"/>
+      <selection pane="bottomRight" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.7109375" style="10" customWidth="1"/>
-    <col min="12" max="23" width="9.140625" style="14" customWidth="1"/>
-    <col min="24" max="36" width="9.140625" style="16"/>
+    <col min="6" max="6" width="21.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.7265625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7265625" style="10" customWidth="1"/>
+    <col min="12" max="23" width="9.1796875" style="14" customWidth="1"/>
+    <col min="24" max="36" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="44" customFormat="1" ht="30">
+    <row r="1" spans="1:38" s="44" customFormat="1" ht="29">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -10385,7 +10373,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>222</v>
@@ -10458,7 +10446,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>231</v>
@@ -10764,13 +10752,13 @@
         <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I10" s="11">
         <v>1</v>
@@ -10881,7 +10869,7 @@
         <v>231</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I11" s="11">
         <v>2</v>
@@ -10958,13 +10946,13 @@
         <v>20</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I12" s="11">
         <v>1</v>
@@ -11104,7 +11092,7 @@
         <v>20</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>231</v>
@@ -11201,7 +11189,7 @@
         <v>231</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="I15" s="11">
         <v>1</v>
@@ -11359,7 +11347,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>231</v>
@@ -11586,7 +11574,7 @@
         <v>10</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>311</v>
+        <v>381</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>231</v>
@@ -11878,7 +11866,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>231</v>
@@ -12127,7 +12115,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>231</v>
@@ -12200,7 +12188,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>231</v>
@@ -12291,7 +12279,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>314</v>
+        <v>257</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>231</v>
@@ -12447,7 +12435,7 @@
         <v>231</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I31" s="11">
         <v>1</v>
@@ -12520,7 +12508,7 @@
         <v>231</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I32" s="11">
         <v>3</v>
@@ -12735,7 +12723,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>231</v>
@@ -12814,7 +12802,7 @@
         <v>10</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>231</v>
@@ -12905,7 +12893,7 @@
         <v>10</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>231</v>
@@ -12982,7 +12970,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>316</v>
+        <v>210</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>231</v>
@@ -13057,7 +13045,7 @@
         <v>10</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>231</v>
@@ -13130,7 +13118,7 @@
         <v>10</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>231</v>
@@ -13282,13 +13270,13 @@
         <v>20</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I42" s="11">
         <v>1</v>
@@ -13397,7 +13385,7 @@
         <v>231</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I43" s="11">
         <v>1</v>
@@ -13470,7 +13458,7 @@
         <v>231</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I44" s="11">
         <v>3</v>
@@ -13541,13 +13529,13 @@
         <v>20</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>319</v>
+        <v>273</v>
       </c>
       <c r="G45" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I45" s="11">
         <v>3</v>
@@ -13770,13 +13758,13 @@
         <v>20</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I48" s="11">
         <v>1</v>
@@ -13887,7 +13875,7 @@
         <v>231</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I49" s="11">
         <v>2</v>
@@ -13966,7 +13954,7 @@
         <v>231</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I50" s="11">
         <v>2</v>
@@ -14104,7 +14092,7 @@
         <v>20</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>231</v>
@@ -14175,7 +14163,7 @@
         <v>20</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>231</v>
@@ -14416,7 +14404,7 @@
         <v>10</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="G56" s="11" t="s">
         <v>231</v>
@@ -14649,7 +14637,7 @@
         <v>10</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G59" s="11" t="s">
         <v>231</v>
@@ -14880,7 +14868,7 @@
         <v>10</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>231</v>
@@ -14951,7 +14939,7 @@
         <v>10</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G63" s="11" t="s">
         <v>231</v>
@@ -15253,13 +15241,13 @@
         <v>20</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="G67" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="I67" s="11">
         <v>1</v>
@@ -15344,7 +15332,7 @@
         <v>20</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>231</v>
@@ -15488,7 +15476,7 @@
         <v>10</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>231</v>
@@ -15586,13 +15574,13 @@
         <v>10</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="I71" s="11">
         <v>1</v>
@@ -15673,7 +15661,7 @@
         <v>10</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>231</v>
@@ -15746,7 +15734,7 @@
         <v>10</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G73" s="11" t="s">
         <v>231</v>
@@ -16257,13 +16245,13 @@
         <v>10</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="I80" s="11">
         <v>1</v>
@@ -16344,13 +16332,13 @@
         <v>10</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>231</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I81" s="11">
         <v>5</v>
@@ -16417,7 +16405,7 @@
         <v>10</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>231</v>
@@ -16632,7 +16620,7 @@
         <v>10</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>231</v>
@@ -16784,7 +16772,7 @@
         <v>10</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="G87" s="11" t="s">
         <v>231</v>
@@ -16946,7 +16934,7 @@
         <v>10</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>231</v>
@@ -17017,7 +17005,7 @@
         <v>10</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>231</v>
@@ -17088,7 +17076,7 @@
         <v>10</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>231</v>
@@ -17140,7 +17128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:38" ht="28.5">
+    <row r="92" spans="1:38">
       <c r="A92" s="8" t="s">
         <v>21</v>
       </c>
@@ -17211,7 +17199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:38" ht="28.5">
+    <row r="93" spans="1:38">
       <c r="A93" s="8" t="s">
         <v>21</v>
       </c>
@@ -17301,13 +17289,13 @@
         <v>20</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>222</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="I94" s="11">
         <v>1</v>
@@ -17392,7 +17380,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>231</v>
@@ -17680,7 +17668,7 @@
         <v>10</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G99" s="11" t="s">
         <v>231</v>
@@ -17822,7 +17810,7 @@
         <v>10</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>231</v>
@@ -17893,7 +17881,7 @@
         <v>10</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>231</v>
@@ -17966,7 +17954,7 @@
         <v>10</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>231</v>
@@ -18524,7 +18512,7 @@
         <v>30</v>
       </c>
       <c r="F110" s="13" t="s">
-        <v>328</v>
+        <v>380</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>231</v>
@@ -18672,7 +18660,7 @@
         <v>30</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>329</v>
+        <v>358</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>231</v>
@@ -18820,7 +18808,7 @@
         <v>10</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>231</v>
@@ -19063,7 +19051,7 @@
         <v>10</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G117" s="11" t="s">
         <v>231</v>
@@ -19207,7 +19195,7 @@
         <v>10</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>231</v>
@@ -19367,7 +19355,7 @@
         <v>10</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>222</v>
@@ -19454,7 +19442,7 @@
         <v>10</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>231</v>
@@ -19525,7 +19513,7 @@
         <v>10</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>231</v>
@@ -19669,7 +19657,7 @@
         <v>10</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>231</v>
@@ -19981,7 +19969,7 @@
         <v>10</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>231</v>
@@ -20216,7 +20204,7 @@
         <v>10</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="G132" s="11" t="s">
         <v>231</v>
@@ -20297,7 +20285,7 @@
         <v>10</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="G133" s="11" t="s">
         <v>231</v>
@@ -20591,7 +20579,7 @@
         <v>10</v>
       </c>
       <c r="F137" s="12" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="G137" s="11" t="s">
         <v>231</v>
@@ -20755,7 +20743,7 @@
         <v>10</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G139" s="11" t="s">
         <v>231</v>
@@ -20846,7 +20834,7 @@
         <v>10</v>
       </c>
       <c r="F140" s="12" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="G140" s="11" t="s">
         <v>231</v>
@@ -21134,7 +21122,7 @@
         <v>10</v>
       </c>
       <c r="F144" s="12" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="G144" s="11" t="s">
         <v>231</v>
@@ -21205,7 +21193,7 @@
         <v>10</v>
       </c>
       <c r="F145" s="12" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="G145" s="11" t="s">
         <v>231</v>
@@ -21473,7 +21461,7 @@
         <v>60</v>
       </c>
       <c r="F148" s="11" t="s">
-        <v>331</v>
+        <v>379</v>
       </c>
       <c r="G148" s="11" t="s">
         <v>231</v>
@@ -21546,7 +21534,7 @@
         <v>60</v>
       </c>
       <c r="F149" s="11" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="G149" s="11" t="s">
         <v>231</v>
@@ -21692,7 +21680,7 @@
         <v>60</v>
       </c>
       <c r="F151" s="11" t="s">
-        <v>332</v>
+        <v>378</v>
       </c>
       <c r="G151" s="11" t="s">
         <v>231</v>
@@ -21838,7 +21826,7 @@
         <v>60</v>
       </c>
       <c r="F153" s="37" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="G153" s="11" t="s">
         <v>231</v>
@@ -22197,7 +22185,7 @@
         <v>10</v>
       </c>
       <c r="F158" s="11" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="G158" s="11" t="s">
         <v>231</v>
@@ -22286,7 +22274,7 @@
         <v>10</v>
       </c>
       <c r="F159" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="G159" s="11" t="s">
         <v>231</v>
@@ -22375,7 +22363,7 @@
         <v>10</v>
       </c>
       <c r="F160" s="11" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="G160" s="11" t="s">
         <v>231</v>
@@ -22446,7 +22434,7 @@
         <v>20</v>
       </c>
       <c r="F161" s="11" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="G161" s="11" t="s">
         <v>231</v>
@@ -22517,7 +22505,7 @@
         <v>20</v>
       </c>
       <c r="F162" s="11" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="G162" s="11" t="s">
         <v>231</v>
@@ -22588,7 +22576,7 @@
         <v>20</v>
       </c>
       <c r="F163" s="11" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="G163" s="11" t="s">
         <v>231</v>
@@ -22659,7 +22647,7 @@
         <v>20</v>
       </c>
       <c r="F164" s="11" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="G164" s="11" t="s">
         <v>231</v>
@@ -22732,7 +22720,7 @@
         <v>20</v>
       </c>
       <c r="F165" s="11" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="G165" s="11" t="s">
         <v>231</v>
@@ -22805,7 +22793,7 @@
         <v>20</v>
       </c>
       <c r="F166" s="11" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="G166" s="11" t="s">
         <v>231</v>
@@ -22878,7 +22866,7 @@
         <v>20</v>
       </c>
       <c r="F167" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="G167" s="11" t="s">
         <v>231</v>
@@ -22949,7 +22937,7 @@
         <v>20</v>
       </c>
       <c r="F168" s="11" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="G168" s="11" t="s">
         <v>231</v>
@@ -23022,7 +23010,7 @@
         <v>20</v>
       </c>
       <c r="F169" s="11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="G169" s="11" t="s">
         <v>231</v>
@@ -23093,7 +23081,7 @@
         <v>20</v>
       </c>
       <c r="F170" s="11" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="G170" s="11" t="s">
         <v>231</v>
@@ -23170,7 +23158,7 @@
         <v>231</v>
       </c>
       <c r="H171" s="11" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="I171" s="11">
         <v>4</v>
@@ -23241,7 +23229,7 @@
         <v>231</v>
       </c>
       <c r="H172" s="11" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="I172" s="11">
         <v>6</v>
@@ -23519,7 +23507,7 @@
         <v>20</v>
       </c>
       <c r="F176" s="11" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="G176" s="11" t="s">
         <v>231</v>
@@ -23592,7 +23580,7 @@
         <v>20</v>
       </c>
       <c r="F177" s="11" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="G177" s="11" t="s">
         <v>231</v>
@@ -23665,7 +23653,7 @@
         <v>20</v>
       </c>
       <c r="F178" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="G178" s="11" t="s">
         <v>231</v>
@@ -23740,16 +23728,16 @@
       <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
-    <col min="7" max="15" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="8.7109375" style="16"/>
+    <col min="6" max="6" width="10.7265625" style="10" customWidth="1"/>
+    <col min="7" max="15" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="17.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -27071,7 +27059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="28.5">
+    <row r="36" spans="1:31">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -29895,18 +29883,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D548CE7-BEAC-43FA-847F-FDE82E3A5926}">
   <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="T74" sqref="T74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="5" customWidth="1"/>
   </cols>
@@ -31720,7 +31708,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="28.5">
+    <row r="36" spans="1:23">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -35335,11 +35323,11 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
change to PX3141 & PX3155
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1656" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C133DB0C-B249-4B27-8DCF-17BA242244FC}"/>
+  <xr:revisionPtr revIDLastSave="1659" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90771DB5-2E25-4391-8958-F86A5E011A76}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -9075,7 +9075,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9993,10 +9993,10 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H82" sqref="H82"/>
+      <selection pane="bottomRight" activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15426,11 +15426,11 @@
       <c r="N69" s="19"/>
       <c r="O69" s="19"/>
       <c r="P69" s="19"/>
-      <c r="Q69" s="19">
+      <c r="Q69" s="19"/>
+      <c r="R69" s="19"/>
+      <c r="S69" s="19">
         <v>0.1</v>
       </c>
-      <c r="R69" s="19"/>
-      <c r="S69" s="19"/>
       <c r="T69" s="19"/>
       <c r="U69" s="18"/>
       <c r="V69" s="18"/>
@@ -16484,7 +16484,7 @@
         <v>231</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I83" s="11">
         <v>4</v>

</xml_diff>

<commit_message>
PX3243 & PX4221 edits
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1706" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43B9F2E6-4A06-47F5-969A-25A16216E35F}"/>
+  <xr:revisionPtr revIDLastSave="1710" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A47FA5FF-87D4-4014-98E7-97A211EE0BFD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="26115" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -9964,27 +9964,27 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF22" sqref="AF22"/>
+      <selection pane="bottomRight" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.7109375" style="10" customWidth="1"/>
-    <col min="12" max="23" width="9.140625" style="14" customWidth="1"/>
-    <col min="24" max="36" width="9.140625" style="16"/>
+    <col min="6" max="6" width="21.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.73046875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.73046875" style="10" customWidth="1"/>
+    <col min="12" max="23" width="9.1328125" style="14" customWidth="1"/>
+    <col min="24" max="36" width="9.1328125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="44" customFormat="1" ht="30">
+    <row r="1" spans="1:38" s="44" customFormat="1" ht="28.5">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -17069,7 +17069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:38" ht="28.5">
+    <row r="92" spans="1:38">
       <c r="A92" s="8" t="s">
         <v>21</v>
       </c>
@@ -17140,7 +17140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:38" ht="28.5">
+    <row r="93" spans="1:38">
       <c r="A93" s="8" t="s">
         <v>21</v>
       </c>
@@ -17544,7 +17544,7 @@
         <v>231</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="I98" s="11">
         <v>4</v>
@@ -19768,7 +19768,7 @@
         <v>231</v>
       </c>
       <c r="H127" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I127" s="11">
         <v>3</v>
@@ -20544,9 +20544,7 @@
       <c r="U137" s="18"/>
       <c r="V137" s="18"/>
       <c r="W137" s="19"/>
-      <c r="X137" s="20">
-        <v>0.01</v>
-      </c>
+      <c r="X137" s="20"/>
       <c r="Y137" s="20">
         <v>0.01</v>
       </c>
@@ -20574,7 +20572,9 @@
       <c r="AG137" s="20">
         <v>0.01</v>
       </c>
-      <c r="AH137" s="20"/>
+      <c r="AH137" s="20">
+        <v>0.01</v>
+      </c>
       <c r="AI137" s="20"/>
       <c r="AJ137" s="20"/>
       <c r="AK137" s="27">
@@ -23664,16 +23664,16 @@
       <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
-    <col min="7" max="15" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="8.7109375" style="16"/>
+    <col min="6" max="6" width="10.73046875" style="10" customWidth="1"/>
+    <col min="7" max="15" width="16.265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="17.265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="8.73046875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -26995,7 +26995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="28.5">
+    <row r="36" spans="1:31">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -29824,14 +29824,14 @@
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.265625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="5" customWidth="1"/>
   </cols>
@@ -31645,7 +31645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="28.5">
+    <row r="36" spans="1:23">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -35261,11 +35261,11 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
date changes for PX3243, PX3253, PX3256
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1710" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A47FA5FF-87D4-4014-98E7-97A211EE0BFD}"/>
+  <xr:revisionPtr revIDLastSave="1713" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15B40F84-9E68-4883-BCAF-AA9C16BA3DEC}"/>
   <bookViews>
     <workbookView xWindow="28702" yWindow="-98" windowWidth="26115" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
@@ -9964,10 +9964,10 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F98" sqref="F98"/>
+      <selection pane="bottomRight" activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -17615,7 +17615,7 @@
         <v>231</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="I99" s="11">
         <v>2</v>
@@ -17901,7 +17901,7 @@
         <v>231</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="I103" s="11">
         <v>11</v>
@@ -18189,7 +18189,7 @@
         <v>231</v>
       </c>
       <c r="H107" s="11" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="I107" s="11">
         <v>4</v>

</xml_diff>

<commit_message>
date changes for PX2232 and PX4230
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2526_v2.xlsx
+++ b/AssessmentSchedule_2526_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1713" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15B40F84-9E68-4883-BCAF-AA9C16BA3DEC}"/>
+  <xr:revisionPtr revIDLastSave="1716" documentId="8_{10702854-9EE2-4D67-90CE-85FDD07A66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49EEAAE0-471A-47C0-9AB3-B72E4BBA97EE}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="26115" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -9964,27 +9964,27 @@
   <dimension ref="A1:AL178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H103" sqref="H103"/>
+      <selection pane="bottomRight" activeCell="AF55" sqref="AF55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.73046875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.73046875" style="10" customWidth="1"/>
-    <col min="12" max="23" width="9.1328125" style="14" customWidth="1"/>
-    <col min="24" max="36" width="9.1328125" style="16"/>
+    <col min="6" max="6" width="21.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" style="10" customWidth="1"/>
+    <col min="12" max="23" width="9.140625" style="14" customWidth="1"/>
+    <col min="24" max="36" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="44" customFormat="1" ht="28.5">
+    <row r="1" spans="1:38" s="44" customFormat="1" ht="30">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -14310,10 +14310,10 @@
       </c>
       <c r="AD55" s="20"/>
       <c r="AE55" s="20"/>
-      <c r="AF55" s="20">
+      <c r="AF55" s="20"/>
+      <c r="AG55" s="20">
         <v>0.1</v>
       </c>
-      <c r="AG55" s="20"/>
       <c r="AH55" s="20"/>
       <c r="AI55" s="20"/>
       <c r="AJ55" s="20"/>
@@ -17069,7 +17069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:38" ht="28.5">
       <c r="A92" s="8" t="s">
         <v>21</v>
       </c>
@@ -17140,7 +17140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:38" ht="28.5">
       <c r="A93" s="8" t="s">
         <v>21</v>
       </c>
@@ -19910,7 +19910,7 @@
         <v>231</v>
       </c>
       <c r="H129" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I129" s="11">
         <v>1</v>
@@ -23664,16 +23664,16 @@
       <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" style="10" customWidth="1"/>
-    <col min="7" max="15" width="16.265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17.265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="30" width="8.73046875" style="16"/>
+    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
+    <col min="7" max="15" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="17.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="8.7109375" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -26995,7 +26995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" ht="28.5">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -29824,14 +29824,14 @@
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.86328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="5" customWidth="1"/>
   </cols>
@@ -31645,7 +31645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" ht="28.5">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -35261,11 +35261,11 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.59765625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">

</xml_diff>